<commit_message>
scissor has been stripped down; it will be rebuilt. (#57) leveller: #55 adding low shelf / high shelf options, other refinements. leveller: better GUI with enable/disabled et al. biquad filter adding shelving options, some optimizations DecibelsToLinear now uses exp instead of pow; supposedly much faster Maj7Width: better param range of rotation lots of keyboard & focus tweaks #40 no longer resizing to fill parent window, a Renoise fix #58
</commit_message>
<xml_diff>
--- a/sizework20240216.xlsx
+++ b/sizework20240216.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\root\git\thenfour\WaveSabre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98883FCD-EB34-461C-BA71-161D725E3D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115ACADD-41F8-48E4-A432-648F663EE1BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25490" yWindow="-2490" windowWidth="25820" windowHeight="14020" xr2:uid="{0D8D836A-3D74-4865-ACF1-B299F3391987}"/>
+    <workbookView xWindow="8760" yWindow="315" windowWidth="19755" windowHeight="14190" xr2:uid="{0D8D836A-3D74-4865-ACF1-B299F3391987}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="20">
   <si>
     <t>maj7</t>
   </si>
@@ -73,6 +73,18 @@
   </si>
   <si>
     <t>filter static letters</t>
+  </si>
+  <si>
+    <t>static init of maj7width</t>
+  </si>
+  <si>
+    <t>adding features to maj7width-</t>
+  </si>
+  <si>
+    <t>scissor</t>
+  </si>
+  <si>
+    <t>all</t>
   </si>
 </sst>
 </file>
@@ -442,190 +454,190 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42744DFF-29C6-4607-B762-3C0E4A9DE2B2}">
-  <dimension ref="A1:N35"/>
+  <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="H2">
+    <row r="2" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I2">
         <v>14912</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>7144</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3">
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3">
         <v>23192</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>8752</v>
       </c>
-      <c r="J3">
-        <f>I3-$I$2</f>
+      <c r="K3">
+        <f>J3-$J$2</f>
         <v>1608</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4">
         <v>23192</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>8992</v>
       </c>
-      <c r="J4">
-        <f t="shared" ref="J4:J17" si="0">I4-$I$2</f>
+      <c r="K4">
+        <f t="shared" ref="K4:K17" si="0">J4-$J$2</f>
         <v>1848</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5">
+    <row r="5" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5">
         <v>23192</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>9080</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <f t="shared" si="0"/>
         <v>1936</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="F6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6">
         <v>23192</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>9284</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <f t="shared" si="0"/>
         <v>2140</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="G7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7">
         <v>23192</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>8760</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <f t="shared" si="0"/>
         <v>1616</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>44080</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>17304</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <f t="shared" si="0"/>
         <v>10160</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9">
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9">
         <v>44080</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>17516</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <f t="shared" si="0"/>
         <v>10372</v>
       </c>
-      <c r="K9">
-        <f>J3+J8</f>
+      <c r="L9">
+        <f>K3+K8</f>
         <v>11768</v>
       </c>
-      <c r="L9">
-        <f>K9-J9</f>
+      <c r="M9">
+        <f>L9-K9</f>
         <v>1396</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" t="s">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
         <v>6</v>
       </c>
       <c r="F10" t="s">
@@ -634,29 +646,29 @@
       <c r="G10" t="s">
         <v>6</v>
       </c>
-      <c r="H10">
+      <c r="H10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10">
         <v>27288</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>11072</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <f t="shared" si="0"/>
         <v>3928</v>
       </c>
-      <c r="K10">
-        <f>J4+J5+J6+J7</f>
+      <c r="L10">
+        <f>K4+K5+K6+K7</f>
         <v>7540</v>
       </c>
-      <c r="L10">
-        <f>K10-J10</f>
+      <c r="M10">
+        <f>L10-K10</f>
         <v>3612</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
         <v>6</v>
       </c>
@@ -669,36 +681,36 @@
       <c r="G11" t="s">
         <v>6</v>
       </c>
-      <c r="H11">
+      <c r="H11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11">
         <v>27288</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>11340</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <f t="shared" si="0"/>
         <v>4196</v>
       </c>
-      <c r="K11">
-        <f>J4+J5+J6+J7+J3</f>
+      <c r="L11">
+        <f>K4+K5+K6+K7+K3</f>
         <v>9148</v>
       </c>
-      <c r="L11">
-        <f>K11-J11</f>
+      <c r="M11">
+        <f>L11-K11</f>
         <v>4952</v>
       </c>
-      <c r="M11">
-        <f>$I$12-I11</f>
+      <c r="N11">
+        <f>$J$12-J11</f>
         <v>8516</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>6</v>
       </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
       <c r="D12" t="s">
         <v>6</v>
       </c>
@@ -711,36 +723,36 @@
       <c r="G12" t="s">
         <v>6</v>
       </c>
-      <c r="H12">
+      <c r="H12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12">
         <v>48176</v>
       </c>
-      <c r="I12" s="2">
+      <c r="J12">
         <v>19856</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <f t="shared" si="0"/>
         <v>12712</v>
       </c>
-      <c r="K12">
-        <f>K11+J8</f>
+      <c r="L12">
+        <f>L11+K8</f>
         <v>19308</v>
       </c>
-      <c r="L12">
-        <f>K12-J12</f>
+      <c r="M12">
+        <f>L12-K12</f>
         <v>6596</v>
       </c>
-      <c r="M12">
-        <f>$I$12</f>
+      <c r="N12">
+        <f>$J$12</f>
         <v>19856</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>6</v>
       </c>
-      <c r="D13" t="s">
-        <v>6</v>
-      </c>
       <c r="E13" t="s">
         <v>6</v>
       </c>
@@ -750,37 +762,37 @@
       <c r="G13" t="s">
         <v>6</v>
       </c>
-      <c r="H13">
+      <c r="H13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13">
         <v>48176</v>
       </c>
-      <c r="I13">
+      <c r="J13">
         <v>19332</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <f t="shared" si="0"/>
         <v>12188</v>
       </c>
-      <c r="K13">
-        <f>K12-J4</f>
+      <c r="L13">
+        <f>L12-K4</f>
         <v>17460</v>
       </c>
-      <c r="L13">
-        <f t="shared" ref="L13:L17" si="1">K13-J13</f>
+      <c r="M13">
+        <f t="shared" ref="M13:M17" si="1">L13-K13</f>
         <v>5272</v>
       </c>
-      <c r="M13">
-        <f>$I$12-I13</f>
+      <c r="N13">
+        <f>$J$12-J13</f>
         <v>524</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>6</v>
       </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="D14" t="s">
         <v>6</v>
       </c>
       <c r="F14" t="s">
@@ -789,114 +801,114 @@
       <c r="G14" t="s">
         <v>6</v>
       </c>
-      <c r="H14">
+      <c r="H14" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14">
         <v>48176</v>
       </c>
-      <c r="I14">
+      <c r="J14">
         <v>19668</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <f t="shared" si="0"/>
         <v>12524</v>
       </c>
-      <c r="K14">
-        <f>$K$12-J3</f>
+      <c r="L14">
+        <f>$L$12-K3</f>
         <v>17700</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <f t="shared" si="1"/>
         <v>5176</v>
       </c>
-      <c r="M14">
-        <f t="shared" ref="M14:M17" si="2">$I$12-I14</f>
+      <c r="N14">
+        <f t="shared" ref="N14:N17" si="2">$J$12-J14</f>
         <v>188</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>6</v>
       </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
       <c r="D15" t="s">
         <v>6</v>
       </c>
-      <c r="F15" t="s">
+      <c r="E15" t="s">
         <v>6</v>
       </c>
       <c r="G15" t="s">
         <v>6</v>
       </c>
-      <c r="H15">
+      <c r="H15" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15">
         <v>48176</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <v>19496</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <f t="shared" si="0"/>
         <v>12352</v>
       </c>
-      <c r="K15">
-        <f>$K$12-J5</f>
+      <c r="L15">
+        <f>$L$12-K5</f>
         <v>17372</v>
       </c>
-      <c r="L15">
+      <c r="M15">
         <f t="shared" si="1"/>
         <v>5020</v>
       </c>
-      <c r="M15">
+      <c r="N15">
         <f t="shared" si="2"/>
         <v>360</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>6</v>
       </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
       <c r="D16" t="s">
         <v>6</v>
       </c>
       <c r="E16" t="s">
         <v>6</v>
       </c>
-      <c r="G16" t="s">
-        <v>6</v>
-      </c>
-      <c r="H16">
+      <c r="F16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H16" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16">
         <v>48176</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <v>18940</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <f t="shared" si="0"/>
         <v>11796</v>
       </c>
-      <c r="K16">
-        <f>$K$12-J6</f>
+      <c r="L16">
+        <f>$L$12-K6</f>
         <v>17168</v>
       </c>
-      <c r="L16">
+      <c r="M16">
         <f t="shared" si="1"/>
         <v>5372</v>
       </c>
-      <c r="M16">
+      <c r="N16">
         <f t="shared" si="2"/>
         <v>916</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>6</v>
       </c>
-      <c r="C17" t="s">
-        <v>6</v>
-      </c>
       <c r="D17" t="s">
         <v>6</v>
       </c>
@@ -906,129 +918,212 @@
       <c r="F17" t="s">
         <v>6</v>
       </c>
-      <c r="H17">
+      <c r="G17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17">
         <v>48176</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <v>19448</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <f t="shared" si="0"/>
         <v>12304</v>
       </c>
-      <c r="K17">
-        <f>$K$12-J7</f>
+      <c r="L17">
+        <f>$L$12-K7</f>
         <v>17692</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <f t="shared" si="1"/>
         <v>5388</v>
       </c>
-      <c r="M17">
+      <c r="N17">
         <f t="shared" si="2"/>
         <v>408</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18">
+        <v>48176</v>
+      </c>
+      <c r="J18" s="2">
+        <v>20036</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19">
+        <v>23192</v>
+      </c>
+      <c r="J19">
+        <v>8564</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>15</v>
       </c>
-      <c r="I20">
+      <c r="J22">
         <v>19700</v>
       </c>
-      <c r="J20">
-        <f>$I$12-I20</f>
+      <c r="K22">
+        <f>$J$12-J22</f>
         <v>156</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F29" t="s">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="J23">
+        <v>19680</v>
+      </c>
+      <c r="K23">
+        <f>$J$12-J23</f>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="J24">
+        <v>19728</v>
+      </c>
+      <c r="K24">
+        <f>$J$12-J24</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
         <v>14</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H31" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E30" t="s">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
         <v>0</v>
       </c>
-      <c r="F30">
-        <f>J8</f>
+      <c r="G32">
+        <f>K8</f>
         <v>10160</v>
       </c>
-      <c r="G30">
-        <f>M11</f>
+      <c r="H32">
+        <f>N11</f>
         <v>8516</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E31" t="s">
+    <row r="33" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
         <v>1</v>
       </c>
-      <c r="F31">
-        <f>J4</f>
+      <c r="G33">
+        <f>K4</f>
         <v>1848</v>
       </c>
-      <c r="G31">
-        <f>M13</f>
+      <c r="H33">
+        <f>N13</f>
         <v>524</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E32" t="s">
+    <row r="34" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
         <v>2</v>
       </c>
-      <c r="F32">
-        <f>J3</f>
+      <c r="G34">
+        <f>K3</f>
         <v>1608</v>
       </c>
-      <c r="G32">
-        <f>M14</f>
+      <c r="H34">
+        <f>N14</f>
         <v>188</v>
       </c>
     </row>
-    <row r="33" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E33" t="s">
+    <row r="35" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
         <v>3</v>
       </c>
-      <c r="F33">
-        <f>J5</f>
+      <c r="G35">
+        <f>K5</f>
         <v>1936</v>
       </c>
-      <c r="G33">
-        <f>M15</f>
+      <c r="H35">
+        <f>N15</f>
         <v>360</v>
       </c>
     </row>
-    <row r="34" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E34" t="s">
+    <row r="36" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
         <v>4</v>
       </c>
-      <c r="F34">
-        <f>J6</f>
+      <c r="G36">
+        <f>K6</f>
         <v>2140</v>
       </c>
-      <c r="G34">
-        <f>M16</f>
+      <c r="H36">
+        <f>N16</f>
         <v>916</v>
       </c>
     </row>
-    <row r="35" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E35" t="s">
+    <row r="37" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
         <v>5</v>
       </c>
-      <c r="F35">
-        <f>J7</f>
+      <c r="G37">
+        <f>K7</f>
         <v>1616</v>
       </c>
-      <c r="G35">
-        <f>M17</f>
+      <c r="H37">
+        <f>N17</f>
         <v>408</v>
       </c>
     </row>
+    <row r="38" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F38" t="s">
+        <v>18</v>
+      </c>
+      <c r="G38">
+        <f>J19-J2</f>
+        <v>1420</v>
+      </c>
+      <c r="H38">
+        <f>J18-J12</f>
+        <v>180</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="H1:I1048576">
+  <conditionalFormatting sqref="I1:J1048576">
     <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="min"/>
@@ -1042,7 +1137,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1:J1048576">
+  <conditionalFormatting sqref="K1:K1048576">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -1072,7 +1167,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H1:I1048576</xm:sqref>
+          <xm:sqref>I1:J1048576</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{F0378A81-E1AD-4E80-A0DF-5687C75C7133}">
@@ -1085,7 +1180,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>J1:J1048576</xm:sqref>
+          <xm:sqref>K1:K1048576</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Maj7 Sat is functional. a multiband saturator.
</commit_message>
<xml_diff>
--- a/sizework20240216.xlsx
+++ b/sizework20240216.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\root\git\thenfour\WaveSabre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115ACADD-41F8-48E4-A432-648F663EE1BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7374054B-C896-483E-BC97-28A88F58203D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8760" yWindow="315" windowWidth="19755" windowHeight="14190" xr2:uid="{0D8D836A-3D74-4865-ACF1-B299F3391987}"/>
+    <workbookView xWindow="12270" yWindow="1020" windowWidth="19755" windowHeight="14190" activeTab="1" xr2:uid="{0D8D836A-3D74-4865-ACF1-B299F3391987}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="31">
   <si>
     <t>maj7</t>
   </si>
@@ -85,6 +86,39 @@
   </si>
   <si>
     <t>all</t>
+  </si>
+  <si>
+    <t>adding features to biquad, leveller</t>
+  </si>
+  <si>
+    <t>optimizing biquad</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>what</t>
+  </si>
+  <si>
+    <t>with lp/hp sepa</t>
+  </si>
+  <si>
+    <t>after biquad optimizations and improvements</t>
+  </si>
+  <si>
+    <t>no smasher</t>
+  </si>
+  <si>
+    <t>with maj7comp</t>
+  </si>
+  <si>
+    <t>removing features</t>
+  </si>
+  <si>
+    <t>wtf how did REMOVING features increase size?</t>
+  </si>
+  <si>
+    <t>removing a call to exp2</t>
   </si>
 </sst>
 </file>
@@ -456,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42744DFF-29C6-4607-B762-3C0E4A9DE2B2}">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1021,6 +1055,35 @@
       <c r="K24">
         <f>$J$12-J24</f>
         <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="J25">
+        <v>20000</v>
+      </c>
+      <c r="K25">
+        <f>J24-J25</f>
+        <v>-272</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J26">
+        <v>19920</v>
+      </c>
+      <c r="K26">
+        <f>J25-J26</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>21</v>
+      </c>
+      <c r="J27">
+        <v>19324</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -1186,4 +1249,95 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C05FD92-F64B-46B2-B040-D64C583D254F}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="42.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2">
+        <v>21899</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>21895</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>21899</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5">
+        <v>19324</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <v>17159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7">
+        <v>19868</v>
+      </c>
+      <c r="C7">
+        <f>B7-B6</f>
+        <v>2709</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8">
+        <v>19872</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9">
+        <v>19868</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
tweaks to editors and params fixing cathedral which sounded terrible cathedral & echo now use wet & dry mixes rather than wet-dry mix.
</commit_message>
<xml_diff>
--- a/sizework20240216.xlsx
+++ b/sizework20240216.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\root\git\thenfour\WaveSabre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7B9DE4-08EB-40B8-8A95-4F3EF531B578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF31C1C-8FAE-4A0E-8A40-E413B396EE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12270" yWindow="1020" windowWidth="19755" windowHeight="14190" activeTab="1" xr2:uid="{0D8D836A-3D74-4865-ACF1-B299F3391987}"/>
+    <workbookView xWindow="14880" yWindow="2100" windowWidth="19575" windowHeight="16800" activeTab="1" xr2:uid="{0D8D836A-3D74-4865-ACF1-B299F3391987}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="89">
   <si>
     <t>maj7</t>
   </si>
@@ -115,9 +115,6 @@
     <t>removing features</t>
   </si>
   <si>
-    <t>wtf how did REMOVING features increase size?</t>
-  </si>
-  <si>
     <t>removing a call to exp2</t>
   </si>
   <si>
@@ -158,6 +155,144 @@
   </si>
   <si>
     <t>oh I re-added the maj7 comp features.</t>
+  </si>
+  <si>
+    <t>w/o maj7</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Running Total</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>diff</t>
+  </si>
+  <si>
+    <t>all devices with M7 style param</t>
+  </si>
+  <si>
+    <t>remove rotation from width</t>
+  </si>
+  <si>
+    <t>adding simpler overload of getfrequency()</t>
+  </si>
+  <si>
+    <t>simpler overload of Get01value</t>
+  </si>
+  <si>
+    <t>wtf how did REMOVING features increase size? (I think it was a mistake; calling wrong object)</t>
+  </si>
+  <si>
+    <t>w/o sat.</t>
+  </si>
+  <si>
+    <t>sat is 1.2kb; unacceptable</t>
+  </si>
+  <si>
+    <t>no initialize cathedral values, some tweaks</t>
+  </si>
+  <si>
+    <t>no maj7 obsolete + var tri waveforms</t>
+  </si>
+  <si>
+    <t>simpler sine clip</t>
+  </si>
+  <si>
+    <t>wow that was a lot of savings :x</t>
+  </si>
+  <si>
+    <t>simpler saw</t>
+  </si>
+  <si>
+    <t>with all devices</t>
+  </si>
+  <si>
+    <t>tiny sat optimization moving a multiply</t>
+  </si>
+  <si>
+    <t>disable 48db crossover</t>
+  </si>
+  <si>
+    <t>removing rarely used sat models</t>
+  </si>
+  <si>
+    <t>removing analog support</t>
+  </si>
+  <si>
+    <t>bypassing sat processample</t>
+  </si>
+  <si>
+    <t>bypass distort()</t>
+  </si>
+  <si>
+    <t>removing all div style models</t>
+  </si>
+  <si>
+    <t>different method of stereo proce</t>
+  </si>
+  <si>
+    <t>no mute/solo processing when no selectable stream</t>
+  </si>
+  <si>
+    <t>tiny fix</t>
+  </si>
+  <si>
+    <t>no ms in sat</t>
+  </si>
+  <si>
+    <t>sat is now 840 bytes</t>
+  </si>
+  <si>
+    <t>no sat</t>
+  </si>
+  <si>
+    <t>no cathedral</t>
+  </si>
+  <si>
+    <t>cathedral is 724 bytes</t>
+  </si>
+  <si>
+    <t>"optimised" echo processing</t>
+  </si>
+  <si>
+    <t>inlining the simplest paramaccessors</t>
+  </si>
+  <si>
+    <t>well I tried but cannot get this to be smaller.</t>
+  </si>
+  <si>
+    <t>wow that is bad.</t>
+  </si>
+  <si>
+    <t>echo baseline again</t>
+  </si>
+  <si>
+    <t>absolute best echo optimization; nope.</t>
+  </si>
+  <si>
+    <t>baseline.</t>
+  </si>
+  <si>
+    <t>unifying loaddefaults and get/setparam</t>
+  </si>
+  <si>
+    <t>some fixes after testing</t>
+  </si>
+  <si>
+    <t>comp no full features</t>
+  </si>
+  <si>
+    <t>what was our baseline again</t>
+  </si>
+  <si>
+    <t>worth it</t>
   </si>
 </sst>
 </file>
@@ -1292,10 +1427,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C05FD92-F64B-46B2-B040-D64C583D254F}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1310,6 +1445,9 @@
       <c r="B1" t="s">
         <v>22</v>
       </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -1365,16 +1503,16 @@
         <v>19872</v>
       </c>
       <c r="C8">
-        <f t="shared" ref="C8:C18" si="0">B8-B7</f>
+        <f t="shared" ref="C8:C71" si="0">B8-B7</f>
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9">
         <v>19868</v>
@@ -1386,7 +1524,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10">
         <v>21628</v>
@@ -1398,7 +1536,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11">
         <v>21028</v>
@@ -1408,12 +1546,12 @@
         <v>-600</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12">
         <v>20240</v>
@@ -1425,7 +1563,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13">
         <v>19628</v>
@@ -1435,12 +1573,12 @@
         <v>-612</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14">
         <v>21520</v>
@@ -1452,7 +1590,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15">
         <v>21460</v>
@@ -1464,7 +1602,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16">
         <v>21420</v>
@@ -1476,7 +1614,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B17">
         <v>21308</v>
@@ -1486,12 +1624,12 @@
         <v>-112</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18">
         <v>21436</v>
@@ -1501,7 +1639,574 @@
         <v>128</v>
       </c>
       <c r="D18" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="2">
+        <v>21276</v>
+      </c>
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>-160</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20">
+        <v>21240</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>-36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21">
+        <v>21224</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>-16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22">
+        <v>21220</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23">
+        <v>19976</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>-1244</v>
+      </c>
+      <c r="D23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>52</v>
+      </c>
+      <c r="B24">
+        <v>21220</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25">
+        <v>21180</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>57</v>
+      </c>
+      <c r="B26">
+        <v>21100</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>-80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B27">
+        <v>21000</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="D27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28">
+        <v>20940</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29">
+        <v>19696</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>-1244</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>61</v>
+      </c>
+      <c r="B30">
+        <v>20940</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>1244</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31">
+        <v>20928</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32">
+        <v>20856</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>-72</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33">
+        <v>20680</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>-176</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34">
+        <v>20616</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>-64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35">
+        <v>20344</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>-272</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B36">
+        <v>20616</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>272</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37">
+        <v>20492</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>-124</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>20616</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39">
+        <v>20572</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>-44</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40">
+        <v>20584</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41">
+        <v>20572</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42">
+        <v>20576</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43">
+        <v>20536</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>-40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44">
+        <v>19696</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>-840</v>
+      </c>
+      <c r="D44" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B45">
+        <v>20536</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>840</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46">
+        <v>19812</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>-724</v>
+      </c>
+      <c r="D46" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B47">
+        <v>20536</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>724</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48">
+        <v>20560</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D48" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>78</v>
+      </c>
+      <c r="B49">
+        <v>20644</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="D49" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>81</v>
+      </c>
+      <c r="B50">
+        <v>20536</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>-108</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>82</v>
+      </c>
+      <c r="B51">
+        <v>20548</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>83</v>
+      </c>
+      <c r="B52">
+        <v>20536</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>84</v>
+      </c>
+      <c r="B53">
+        <v>20468</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>-68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>85</v>
+      </c>
+      <c r="B54">
+        <v>20524</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>86</v>
+      </c>
+      <c r="B55">
+        <v>20380</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>-144</v>
+      </c>
+      <c r="D55" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>87</v>
+      </c>
+      <c r="B56" s="2">
+        <v>21276</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>896</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C65">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C66">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C67">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C68">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C69">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C70">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C71">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C72">
+        <f t="shared" ref="C72:C73" si="1">B72-B71</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C73">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
VSTs now show which features have been selectively disabled Maj7 now has an output VU meter removing maj7 oscillator detune & oscillator spread
</commit_message>
<xml_diff>
--- a/sizework20240216.xlsx
+++ b/sizework20240216.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\root\git\thenfour\WaveSabre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF31C1C-8FAE-4A0E-8A40-E413B396EE37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519CDBD7-54BA-44C1-9861-6822E2B4C8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14880" yWindow="2100" windowWidth="19575" windowHeight="16800" activeTab="1" xr2:uid="{0D8D836A-3D74-4865-ACF1-B299F3391987}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="95">
   <si>
     <t>maj7</t>
   </si>
@@ -293,6 +293,24 @@
   </si>
   <si>
     <t>worth it</t>
+  </si>
+  <si>
+    <t>cathedral init code</t>
+  </si>
+  <si>
+    <t>no portamento curve</t>
+  </si>
+  <si>
+    <t>baseline</t>
+  </si>
+  <si>
+    <t>deltafrombase</t>
+  </si>
+  <si>
+    <t>removing osc spread &amp; detune</t>
+  </si>
+  <si>
+    <t>man not much savings</t>
   </si>
 </sst>
 </file>
@@ -316,7 +334,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -326,6 +344,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -342,12 +366,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1427,29 +1452,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C05FD92-F64B-46B2-B040-D64C583D254F}">
-  <dimension ref="A1:D73"/>
+  <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1457,17 +1490,17 @@
         <v>21899</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>21895</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>21899</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1475,7 +1508,7 @@
         <v>19324</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1483,7 +1516,7 @@
         <v>17159</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1495,7 +1528,7 @@
         <v>2709</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1506,11 +1539,11 @@
         <f t="shared" ref="C8:C71" si="0">B8-B7</f>
         <v>4</v>
       </c>
-      <c r="D8" t="s">
+      <c r="F8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1522,7 +1555,7 @@
         <v>-4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1534,7 +1567,7 @@
         <v>1760</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1545,11 +1578,11 @@
         <f t="shared" si="0"/>
         <v>-600</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1561,7 +1594,7 @@
         <v>-788</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1572,11 +1605,11 @@
         <f t="shared" si="0"/>
         <v>-612</v>
       </c>
-      <c r="D13" t="s">
+      <c r="F13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -1588,7 +1621,7 @@
         <v>1892</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>37</v>
       </c>
@@ -1600,7 +1633,7 @@
         <v>-60</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -1612,7 +1645,7 @@
         <v>-40</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -1623,11 +1656,11 @@
         <f t="shared" si="0"/>
         <v>-112</v>
       </c>
-      <c r="D17" t="s">
+      <c r="F17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>41</v>
       </c>
@@ -1638,11 +1671,11 @@
         <f t="shared" si="0"/>
         <v>128</v>
       </c>
-      <c r="D18" t="s">
+      <c r="F18" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>49</v>
       </c>
@@ -1653,8 +1686,15 @@
         <f t="shared" si="0"/>
         <v>-160</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>21276</v>
+      </c>
+      <c r="E19">
+        <f>B19-D19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -1665,8 +1705,15 @@
         <f t="shared" si="0"/>
         <v>-36</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>21276</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ref="E20:E73" si="1">B20-D20</f>
+        <v>-36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -1677,8 +1724,15 @@
         <f t="shared" si="0"/>
         <v>-16</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>21276</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>-52</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>52</v>
       </c>
@@ -1689,8 +1743,15 @@
         <f t="shared" si="0"/>
         <v>-4</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>21276</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>-56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>54</v>
       </c>
@@ -1701,11 +1762,18 @@
         <f t="shared" si="0"/>
         <v>-1244</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23">
+        <v>21276</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>-1300</v>
+      </c>
+      <c r="F23" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -1716,8 +1784,15 @@
         <f t="shared" si="0"/>
         <v>1244</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>21276</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>-56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -1728,8 +1803,15 @@
         <f t="shared" si="0"/>
         <v>-40</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>21276</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>-96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>57</v>
       </c>
@@ -1740,8 +1822,15 @@
         <f t="shared" si="0"/>
         <v>-80</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>21276</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>-176</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -1752,11 +1841,18 @@
         <f t="shared" si="0"/>
         <v>-100</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27">
+        <v>21276</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="1"/>
+        <v>-276</v>
+      </c>
+      <c r="F27" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -1767,8 +1863,15 @@
         <f t="shared" si="0"/>
         <v>-60</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>21276</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="1"/>
+        <v>-336</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>54</v>
       </c>
@@ -1779,8 +1882,15 @@
         <f t="shared" si="0"/>
         <v>-1244</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D29">
+        <v>21276</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="1"/>
+        <v>-1580</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>61</v>
       </c>
@@ -1791,8 +1901,15 @@
         <f t="shared" si="0"/>
         <v>1244</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D30">
+        <v>21276</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>-336</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>62</v>
       </c>
@@ -1803,8 +1920,15 @@
         <f t="shared" si="0"/>
         <v>-12</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>21276</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="1"/>
+        <v>-348</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -1815,8 +1939,15 @@
         <f t="shared" si="0"/>
         <v>-72</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>21276</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="1"/>
+        <v>-420</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>64</v>
       </c>
@@ -1827,8 +1958,15 @@
         <f t="shared" si="0"/>
         <v>-176</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>21276</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="1"/>
+        <v>-596</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>65</v>
       </c>
@@ -1839,8 +1977,15 @@
         <f t="shared" si="0"/>
         <v>-64</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>21276</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="1"/>
+        <v>-660</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>66</v>
       </c>
@@ -1851,8 +1996,15 @@
         <f t="shared" si="0"/>
         <v>-272</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>21276</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="1"/>
+        <v>-932</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>20616</v>
       </c>
@@ -1860,8 +2012,15 @@
         <f t="shared" si="0"/>
         <v>272</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>21276</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="1"/>
+        <v>-660</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>67</v>
       </c>
@@ -1872,8 +2031,15 @@
         <f t="shared" si="0"/>
         <v>-124</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>21276</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="1"/>
+        <v>-784</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B38">
         <v>20616</v>
       </c>
@@ -1881,8 +2047,15 @@
         <f t="shared" si="0"/>
         <v>124</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>21276</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="1"/>
+        <v>-660</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>68</v>
       </c>
@@ -1893,8 +2066,15 @@
         <f t="shared" si="0"/>
         <v>-44</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>21276</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="1"/>
+        <v>-704</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>69</v>
       </c>
@@ -1905,8 +2085,15 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>21276</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="1"/>
+        <v>-692</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>70</v>
       </c>
@@ -1917,8 +2104,15 @@
         <f t="shared" si="0"/>
         <v>-12</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>21276</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="1"/>
+        <v>-704</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>71</v>
       </c>
@@ -1929,8 +2123,15 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>21276</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="1"/>
+        <v>-700</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>72</v>
       </c>
@@ -1941,8 +2142,15 @@
         <f t="shared" si="0"/>
         <v>-40</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>21276</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="1"/>
+        <v>-740</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>74</v>
       </c>
@@ -1953,11 +2161,18 @@
         <f t="shared" si="0"/>
         <v>-840</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44">
+        <v>21276</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="1"/>
+        <v>-1580</v>
+      </c>
+      <c r="F44" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B45">
         <v>20536</v>
       </c>
@@ -1965,8 +2180,15 @@
         <f t="shared" si="0"/>
         <v>840</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>21276</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="1"/>
+        <v>-740</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>75</v>
       </c>
@@ -1977,11 +2199,18 @@
         <f t="shared" si="0"/>
         <v>-724</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46">
+        <v>21276</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="1"/>
+        <v>-1464</v>
+      </c>
+      <c r="F46" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B47">
         <v>20536</v>
       </c>
@@ -1989,8 +2218,15 @@
         <f t="shared" si="0"/>
         <v>724</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>21276</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="1"/>
+        <v>-740</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>77</v>
       </c>
@@ -2001,11 +2237,18 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48">
+        <v>21276</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="1"/>
+        <v>-716</v>
+      </c>
+      <c r="F48" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>78</v>
       </c>
@@ -2016,11 +2259,18 @@
         <f t="shared" si="0"/>
         <v>84</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49">
+        <v>21276</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="1"/>
+        <v>-632</v>
+      </c>
+      <c r="F49" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>81</v>
       </c>
@@ -2031,8 +2281,15 @@
         <f t="shared" si="0"/>
         <v>-108</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <v>21276</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="1"/>
+        <v>-740</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>82</v>
       </c>
@@ -2043,8 +2300,15 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D51">
+        <v>21276</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="1"/>
+        <v>-728</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>83</v>
       </c>
@@ -2055,8 +2319,15 @@
         <f t="shared" si="0"/>
         <v>-12</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D52">
+        <v>21276</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="1"/>
+        <v>-740</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>84</v>
       </c>
@@ -2067,8 +2338,15 @@
         <f t="shared" si="0"/>
         <v>-68</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D53">
+        <v>21276</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="1"/>
+        <v>-808</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>85</v>
       </c>
@@ -2079,8 +2357,15 @@
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D54">
+        <v>21276</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="1"/>
+        <v>-752</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>86</v>
       </c>
@@ -2091,11 +2376,18 @@
         <f t="shared" si="0"/>
         <v>-144</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55">
+        <v>21276</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="1"/>
+        <v>-896</v>
+      </c>
+      <c r="F55" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>87</v>
       </c>
@@ -2106,105 +2398,207 @@
         <f t="shared" si="0"/>
         <v>896</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="2">
+        <v>21276</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>89</v>
+      </c>
+      <c r="B57">
+        <v>20360</v>
+      </c>
       <c r="C57">
         <f t="shared" si="0"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-916</v>
+      </c>
+      <c r="D57">
+        <v>21276</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="1"/>
+        <v>-916</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>90</v>
+      </c>
+      <c r="B58">
+        <v>20348</v>
+      </c>
       <c r="C58">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-12</v>
+      </c>
+      <c r="D58">
+        <v>21276</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="1"/>
+        <v>-928</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>93</v>
+      </c>
+      <c r="B59">
+        <v>20316</v>
+      </c>
       <c r="C59">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-32</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="1"/>
+        <v>20316</v>
+      </c>
+      <c r="F59" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C60">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-20316</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C61">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C62">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C63">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C64">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E64">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C65">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E65">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C66">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E66">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C67">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E67">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C68">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E68">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C69">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E69">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C70">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E70">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C71">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E71">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C72">
-        <f t="shared" ref="C72:C73" si="1">B72-B71</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+        <f t="shared" ref="C72:C73" si="2">B72-B71</f>
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C73">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E73">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
fixed a small crash in project mgr
</commit_message>
<xml_diff>
--- a/sizework20240216.xlsx
+++ b/sizework20240216.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\root\git\thenfour\WaveSabre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{519CDBD7-54BA-44C1-9861-6822E2B4C8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD409A7-9BEF-44CB-AC6A-82F792D67AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14880" yWindow="2100" windowWidth="19575" windowHeight="16800" activeTab="1" xr2:uid="{0D8D836A-3D74-4865-ACF1-B299F3391987}"/>
+    <workbookView xWindow="19740" yWindow="-60" windowWidth="19575" windowHeight="16800" activeTab="1" xr2:uid="{0D8D836A-3D74-4865-ACF1-B299F3391987}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="98">
   <si>
     <t>maj7</t>
   </si>
@@ -311,6 +311,15 @@
   </si>
   <si>
     <t>man not much savings</t>
+  </si>
+  <si>
+    <t>tiny fixes</t>
+  </si>
+  <si>
+    <t>#61 track directive support</t>
+  </si>
+  <si>
+    <t>at least it was a tiny change</t>
   </si>
 </sst>
 </file>
@@ -1455,8 +1464,8 @@
   <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F60" sqref="F60"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2455,42 +2464,69 @@
         <f t="shared" si="0"/>
         <v>-32</v>
       </c>
+      <c r="D59">
+        <v>21276</v>
+      </c>
       <c r="E59">
         <f t="shared" si="1"/>
-        <v>20316</v>
+        <v>-960</v>
       </c>
       <c r="F59" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>95</v>
+      </c>
+      <c r="B60">
+        <v>20304</v>
+      </c>
       <c r="C60">
         <f t="shared" si="0"/>
-        <v>-20316</v>
+        <v>-12</v>
+      </c>
+      <c r="D60">
+        <v>21276</v>
       </c>
       <c r="E60">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-972</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>96</v>
+      </c>
+      <c r="B61">
+        <v>20312</v>
+      </c>
       <c r="C61">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="D61">
+        <v>21276</v>
       </c>
       <c r="E61">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-964</v>
+      </c>
+      <c r="F61" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C62">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-20312</v>
+      </c>
+      <c r="D62">
+        <v>21276</v>
       </c>
       <c r="E62">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-21276</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -2498,9 +2534,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="D63">
+        <v>21276</v>
+      </c>
       <c r="E63">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-21276</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -2508,9 +2547,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="D64">
+        <v>21276</v>
+      </c>
       <c r="E64">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-21276</v>
       </c>
     </row>
     <row r="65" spans="3:5" x14ac:dyDescent="0.25">
@@ -2518,9 +2560,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="D65">
+        <v>21276</v>
+      </c>
       <c r="E65">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-21276</v>
       </c>
     </row>
     <row r="66" spans="3:5" x14ac:dyDescent="0.25">
@@ -2528,9 +2573,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="D66">
+        <v>21276</v>
+      </c>
       <c r="E66">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-21276</v>
       </c>
     </row>
     <row r="67" spans="3:5" x14ac:dyDescent="0.25">
@@ -2538,9 +2586,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="D67">
+        <v>21276</v>
+      </c>
       <c r="E67">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-21276</v>
       </c>
     </row>
     <row r="68" spans="3:5" x14ac:dyDescent="0.25">
@@ -2548,9 +2599,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="D68">
+        <v>21276</v>
+      </c>
       <c r="E68">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-21276</v>
       </c>
     </row>
     <row r="69" spans="3:5" x14ac:dyDescent="0.25">
@@ -2558,9 +2612,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="D69">
+        <v>21276</v>
+      </c>
       <c r="E69">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-21276</v>
       </c>
     </row>
     <row r="70" spans="3:5" x14ac:dyDescent="0.25">
@@ -2568,9 +2625,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="D70">
+        <v>21276</v>
+      </c>
       <c r="E70">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-21276</v>
       </c>
     </row>
     <row r="71" spans="3:5" x14ac:dyDescent="0.25">
@@ -2578,9 +2638,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="D71">
+        <v>21276</v>
+      </c>
       <c r="E71">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-21276</v>
       </c>
     </row>
     <row r="72" spans="3:5" x14ac:dyDescent="0.25">
@@ -2588,9 +2651,12 @@
         <f t="shared" ref="C72:C73" si="2">B72-B71</f>
         <v>0</v>
       </c>
+      <c r="D72">
+        <v>21276</v>
+      </c>
       <c r="E72">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-21276</v>
       </c>
     </row>
     <row r="73" spans="3:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
removing old WS Q param conversion; reuse the div param better slope / filter captions biquad filter is now an option in Maj7 moog filter is now disableable. it's safer for size to go without. biquad + sat kinda replaces it.
</commit_message>
<xml_diff>
--- a/sizework20240216.xlsx
+++ b/sizework20240216.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\root\git\thenfour\WaveSabre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFD409A7-9BEF-44CB-AC6A-82F792D67AF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51EACF8C-E3D3-42EF-8D30-9C1B3786C3DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19740" yWindow="-60" windowWidth="19575" windowHeight="16800" activeTab="1" xr2:uid="{0D8D836A-3D74-4865-ACF1-B299F3391987}"/>
+    <workbookView xWindow="13500" yWindow="1050" windowWidth="19575" windowHeight="16800" activeTab="1" xr2:uid="{0D8D836A-3D74-4865-ACF1-B299F3391987}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -157,21 +157,6 @@
     <t>oh I re-added the maj7 comp features.</t>
   </si>
   <si>
-    <t>w/o maj7</t>
-  </si>
-  <si>
-    <t>Sum</t>
-  </si>
-  <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
-  </si>
-  <si>
     <t>diff</t>
   </si>
   <si>
@@ -320,6 +305,21 @@
   </si>
   <si>
     <t>at least it was a tiny change</t>
+  </si>
+  <si>
+    <t>adding biquad option, readding onepole, removing moog</t>
+  </si>
+  <si>
+    <t>also removing obsolete param types</t>
+  </si>
+  <si>
+    <t>at this point I have saved well over 1kb, though added</t>
+  </si>
+  <si>
+    <t>removing comp &amp; sat</t>
+  </si>
+  <si>
+    <t>1.4kb via sat &amp; comp. but you can argue I'll save this via directives. So I'm good.</t>
   </si>
 </sst>
 </file>
@@ -1464,8 +1464,8 @@
   <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A61" sqref="A61"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1482,13 +1482,13 @@
         <v>22</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1549,7 +1549,7 @@
         <v>4</v>
       </c>
       <c r="F8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1686,7 +1686,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B19" s="2">
         <v>21276</v>
@@ -1705,7 +1705,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B20">
         <v>21240</v>
@@ -1724,7 +1724,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B21">
         <v>21224</v>
@@ -1743,7 +1743,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B22">
         <v>21220</v>
@@ -1762,7 +1762,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B23">
         <v>19976</v>
@@ -1779,12 +1779,12 @@
         <v>-1300</v>
       </c>
       <c r="F23" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B24">
         <v>21220</v>
@@ -1803,7 +1803,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B25">
         <v>21180</v>
@@ -1822,7 +1822,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B26">
         <v>21100</v>
@@ -1841,7 +1841,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B27">
         <v>21000</v>
@@ -1858,12 +1858,12 @@
         <v>-276</v>
       </c>
       <c r="F27" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B28">
         <v>20940</v>
@@ -1882,7 +1882,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B29">
         <v>19696</v>
@@ -1901,7 +1901,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B30">
         <v>20940</v>
@@ -1920,7 +1920,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B31">
         <v>20928</v>
@@ -1939,7 +1939,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B32">
         <v>20856</v>
@@ -1958,7 +1958,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B33">
         <v>20680</v>
@@ -1977,7 +1977,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B34">
         <v>20616</v>
@@ -1996,7 +1996,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B35">
         <v>20344</v>
@@ -2031,7 +2031,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B37">
         <v>20492</v>
@@ -2066,7 +2066,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B39">
         <v>20572</v>
@@ -2085,7 +2085,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B40">
         <v>20584</v>
@@ -2104,7 +2104,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B41">
         <v>20572</v>
@@ -2123,7 +2123,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B42">
         <v>20576</v>
@@ -2142,7 +2142,7 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B43">
         <v>20536</v>
@@ -2161,7 +2161,7 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B44">
         <v>19696</v>
@@ -2178,7 +2178,7 @@
         <v>-1580</v>
       </c>
       <c r="F44" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2199,7 +2199,7 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B46">
         <v>19812</v>
@@ -2216,7 +2216,7 @@
         <v>-1464</v>
       </c>
       <c r="F46" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2237,7 +2237,7 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B48">
         <v>20560</v>
@@ -2254,12 +2254,12 @@
         <v>-716</v>
       </c>
       <c r="F48" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B49">
         <v>20644</v>
@@ -2276,12 +2276,12 @@
         <v>-632</v>
       </c>
       <c r="F49" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B50">
         <v>20536</v>
@@ -2300,7 +2300,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B51">
         <v>20548</v>
@@ -2319,7 +2319,7 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B52">
         <v>20536</v>
@@ -2338,7 +2338,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B53">
         <v>20468</v>
@@ -2357,7 +2357,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B54">
         <v>20524</v>
@@ -2376,7 +2376,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B55">
         <v>20380</v>
@@ -2393,12 +2393,12 @@
         <v>-896</v>
       </c>
       <c r="F55" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B56" s="2">
         <v>21276</v>
@@ -2417,7 +2417,7 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B57">
         <v>20360</v>
@@ -2436,7 +2436,7 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B58">
         <v>20348</v>
@@ -2455,7 +2455,7 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B59">
         <v>20316</v>
@@ -2472,12 +2472,12 @@
         <v>-960</v>
       </c>
       <c r="F59" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B60">
         <v>20304</v>
@@ -2496,7 +2496,7 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B61">
         <v>20312</v>
@@ -2513,52 +2513,76 @@
         <v>-964</v>
       </c>
       <c r="F61" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>93</v>
+      </c>
+      <c r="B62">
+        <v>20172</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>-140</v>
+      </c>
+      <c r="D62">
+        <v>21276</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="1"/>
+        <v>-1104</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>94</v>
+      </c>
+      <c r="B63">
+        <v>20172</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>21276</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="1"/>
+        <v>-1104</v>
+      </c>
+      <c r="F63" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>96</v>
+      </c>
+      <c r="B64">
+        <v>18812</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="0"/>
+        <v>-1360</v>
+      </c>
+      <c r="D64">
+        <v>21276</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="1"/>
+        <v>-2464</v>
+      </c>
+      <c r="F64" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C62">
-        <f t="shared" si="0"/>
-        <v>-20312</v>
-      </c>
-      <c r="D62">
-        <v>21276</v>
-      </c>
-      <c r="E62">
-        <f t="shared" si="1"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C63">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D63">
-        <v>21276</v>
-      </c>
-      <c r="E63">
-        <f t="shared" si="1"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C64">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D64">
-        <v>21276</v>
-      </c>
-      <c r="E64">
-        <f t="shared" si="1"/>
-        <v>-21276</v>
       </c>
     </row>
     <row r="65" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C65">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-18812</v>
       </c>
       <c r="D65">
         <v>21276</v>

</xml_diff>

<commit_message>
maj7sat: shuffling around the selection of models available. trying to balance the uses of saturation
</commit_message>
<xml_diff>
--- a/sizework20240216.xlsx
+++ b/sizework20240216.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\root\git\thenfour\WaveSabre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51EACF8C-E3D3-42EF-8D30-9C1B3786C3DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF7E081-2210-43AB-95AE-0276A35C16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13500" yWindow="1050" windowWidth="19575" windowHeight="16800" activeTab="1" xr2:uid="{0D8D836A-3D74-4865-ACF1-B299F3391987}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="101">
   <si>
     <t>maj7</t>
   </si>
@@ -320,6 +320,15 @@
   </si>
   <si>
     <t>1.4kb via sat &amp; comp. but you can argue I'll save this via directives. So I'm good.</t>
+  </si>
+  <si>
+    <t>readding the div saturation style, removing sin()</t>
+  </si>
+  <si>
+    <t>adding moog filter</t>
+  </si>
+  <si>
+    <t>so yea moog filter consumes 360 bytes of compressed code. Too much to justify as long as biquad exists</t>
   </si>
 </sst>
 </file>
@@ -1465,7 +1474,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F65" sqref="F65"/>
+      <selection pane="bottomLeft" activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2579,98 +2588,116 @@
         <v>97</v>
       </c>
     </row>
-    <row r="65" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B65">
+        <v>20172</v>
+      </c>
       <c r="C65">
         <f t="shared" si="0"/>
-        <v>-18812</v>
+        <v>1360</v>
       </c>
       <c r="D65">
         <v>21276</v>
       </c>
       <c r="E65">
         <f t="shared" si="1"/>
+        <v>-1104</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>98</v>
+      </c>
+      <c r="B66">
+        <v>20232</v>
+      </c>
+      <c r="C66">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="D66">
+        <v>21276</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="1"/>
+        <v>-1044</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>99</v>
+      </c>
+      <c r="B67">
+        <v>20592</v>
+      </c>
+      <c r="C67">
+        <f t="shared" si="0"/>
+        <v>360</v>
+      </c>
+      <c r="D67">
+        <v>21276</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="1"/>
+        <v>-684</v>
+      </c>
+      <c r="F67" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C68">
+        <f t="shared" si="0"/>
+        <v>-20592</v>
+      </c>
+      <c r="D68">
+        <v>21276</v>
+      </c>
+      <c r="E68">
+        <f t="shared" si="1"/>
         <v>-21276</v>
       </c>
     </row>
-    <row r="66" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C66">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C69">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D66">
-        <v>21276</v>
-      </c>
-      <c r="E66">
+      <c r="D69">
+        <v>21276</v>
+      </c>
+      <c r="E69">
         <f t="shared" si="1"/>
         <v>-21276</v>
       </c>
     </row>
-    <row r="67" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C67">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C70">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D67">
-        <v>21276</v>
-      </c>
-      <c r="E67">
+      <c r="D70">
+        <v>21276</v>
+      </c>
+      <c r="E70">
         <f t="shared" si="1"/>
         <v>-21276</v>
       </c>
     </row>
-    <row r="68" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C68">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C71">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D68">
-        <v>21276</v>
-      </c>
-      <c r="E68">
+      <c r="D71">
+        <v>21276</v>
+      </c>
+      <c r="E71">
         <f t="shared" si="1"/>
         <v>-21276</v>
       </c>
     </row>
-    <row r="69" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C69">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D69">
-        <v>21276</v>
-      </c>
-      <c r="E69">
-        <f t="shared" si="1"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="70" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C70">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D70">
-        <v>21276</v>
-      </c>
-      <c r="E70">
-        <f t="shared" si="1"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="71" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C71">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D71">
-        <v>21276</v>
-      </c>
-      <c r="E71">
-        <f t="shared" si="1"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="72" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C72">
         <f t="shared" ref="C72:C73" si="2">B72-B71</f>
         <v>0</v>
@@ -2683,7 +2710,7 @@
         <v>-21276</v>
       </c>
     </row>
-    <row r="73" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C73">
         <f t="shared" si="2"/>
         <v>0</v>

</xml_diff>

<commit_message>
fixed some formatting in maj7 gui now displaying both filters filter types as radio buttons and excluding disabled filter types re-enabling analog option in sat refreshing maj7 defaults: correct filter type, tweak to portamento time
</commit_message>
<xml_diff>
--- a/sizework20240216.xlsx
+++ b/sizework20240216.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\root\git\thenfour\WaveSabre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF7E081-2210-43AB-95AE-0276A35C16EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B03D6E-BBCE-4E15-9C90-5AE7A5EBA09C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13500" yWindow="1050" windowWidth="19575" windowHeight="16800" activeTab="1" xr2:uid="{0D8D836A-3D74-4865-ACF1-B299F3391987}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="103">
   <si>
     <t>maj7</t>
   </si>
@@ -329,6 +329,12 @@
   </si>
   <si>
     <t>so yea moog filter consumes 360 bytes of compressed code. Too much to justify as long as biquad exists</t>
+  </si>
+  <si>
+    <t>adding a tanh folder</t>
+  </si>
+  <si>
+    <t>readding analog</t>
   </si>
 </sst>
 </file>
@@ -1473,8 +1479,8 @@
   <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A57" sqref="A57"/>
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2646,35 +2652,47 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B68">
+        <v>20232</v>
+      </c>
       <c r="C68">
         <f t="shared" si="0"/>
-        <v>-20592</v>
+        <v>-360</v>
       </c>
       <c r="D68">
         <v>21276</v>
       </c>
       <c r="E68">
         <f t="shared" si="1"/>
-        <v>-21276</v>
+        <v>-1044</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>101</v>
+      </c>
+      <c r="B69">
+        <v>20260</v>
+      </c>
       <c r="C69">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="D69">
         <v>21276</v>
       </c>
       <c r="E69">
         <f t="shared" si="1"/>
-        <v>-21276</v>
+        <v>-1016</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>102</v>
+      </c>
       <c r="C70">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-20260</v>
       </c>
       <c r="D70">
         <v>21276</v>

</xml_diff>

<commit_message>
#62: simpler panning basis. same code size, but simpler design. rearranging mod dests to account for the fact that filters are the most modulated thing.
</commit_message>
<xml_diff>
--- a/sizework20240216.xlsx
+++ b/sizework20240216.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\root\git\thenfour\WaveSabre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60B03D6E-BBCE-4E15-9C90-5AE7A5EBA09C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C3A9AE-EE9B-4D49-AFCD-61C99F48F6E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13500" yWindow="1050" windowWidth="19575" windowHeight="16800" activeTab="1" xr2:uid="{0D8D836A-3D74-4865-ACF1-B299F3391987}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="104">
   <si>
     <t>maj7</t>
   </si>
@@ -334,7 +334,10 @@
     <t>adding a tanh folder</t>
   </si>
   <si>
-    <t>readding analog</t>
+    <t>readding analog, making oscillators mono, global modulateable pan</t>
+  </si>
+  <si>
+    <t>I honestly thought making oscillators mono would result in smaller.</t>
   </si>
 </sst>
 </file>
@@ -1480,7 +1483,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A69" sqref="A69"/>
+      <selection pane="bottomLeft" activeCell="A71" sqref="A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2690,22 +2693,28 @@
       <c r="A70" t="s">
         <v>102</v>
       </c>
+      <c r="B70">
+        <v>20276</v>
+      </c>
       <c r="C70">
         <f t="shared" si="0"/>
-        <v>-20260</v>
+        <v>16</v>
       </c>
       <c r="D70">
         <v>21276</v>
       </c>
       <c r="E70">
         <f t="shared" si="1"/>
-        <v>-21276</v>
+        <v>-1000</v>
+      </c>
+      <c r="F70" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C71">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-20276</v>
       </c>
       <c r="D71">
         <v>21276</v>

</xml_diff>

<commit_message>
forcing 24db/oct crossover slope; it's a good balance, saves >200 bytes of code, and crossover slope is really a fringe param. moog filter optimizations moog is BACK.
</commit_message>
<xml_diff>
--- a/sizework20240216.xlsx
+++ b/sizework20240216.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\root\git\thenfour\WaveSabre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9C3A9AE-EE9B-4D49-AFCD-61C99F48F6E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD8D5A7-9945-46CF-82C4-0516D9962F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13500" yWindow="1050" windowWidth="19575" windowHeight="16800" activeTab="1" xr2:uid="{0D8D836A-3D74-4865-ACF1-B299F3391987}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="107">
   <si>
     <t>maj7</t>
   </si>
@@ -338,6 +338,15 @@
   </si>
   <si>
     <t>I honestly thought making oscillators mono would result in smaller.</t>
+  </si>
+  <si>
+    <t>fixes to osc volume mod, removing some calls to floatequals</t>
+  </si>
+  <si>
+    <t>trying moogfilter again</t>
+  </si>
+  <si>
+    <t>some small optimizations to moog; I'm trying to justify bringing it back.</t>
   </si>
 </sst>
 </file>
@@ -1482,8 +1491,8 @@
   <dimension ref="A1:F73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A71" sqref="A71"/>
+      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2712,35 +2721,50 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>104</v>
+      </c>
+      <c r="B71">
+        <v>20276</v>
+      </c>
       <c r="C71">
         <f t="shared" si="0"/>
-        <v>-20276</v>
+        <v>0</v>
       </c>
       <c r="D71">
         <v>21276</v>
       </c>
       <c r="E71">
         <f t="shared" si="1"/>
-        <v>-21276</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>105</v>
+      </c>
+      <c r="B72">
+        <v>20616</v>
+      </c>
       <c r="C72">
         <f t="shared" ref="C72:C73" si="2">B72-B71</f>
-        <v>0</v>
+        <v>340</v>
       </c>
       <c r="D72">
         <v>21276</v>
       </c>
       <c r="E72">
         <f t="shared" si="1"/>
-        <v>-21276</v>
+        <v>-660</v>
+      </c>
+      <c r="F72" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C73">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-20616</v>
       </c>
       <c r="E73">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
adding option to fix amp env modulations which would be broken because of changing enum indices.
</commit_message>
<xml_diff>
--- a/sizework20240216.xlsx
+++ b/sizework20240216.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\root\git\thenfour\WaveSabre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD8D5A7-9945-46CF-82C4-0516D9962F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8176A4-FEF8-4A7B-92AC-F0E938F317C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13500" yWindow="1050" windowWidth="19575" windowHeight="16800" activeTab="1" xr2:uid="{0D8D836A-3D74-4865-ACF1-B299F3391987}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="109">
   <si>
     <t>maj7</t>
   </si>
@@ -347,6 +347,12 @@
   </si>
   <si>
     <t>some small optimizations to moog; I'm trying to justify bringing it back.</t>
+  </si>
+  <si>
+    <t>sat: no slope option at all (24db/oct forced)</t>
+  </si>
+  <si>
+    <t>ok now we're talking. Moog is back baby</t>
   </si>
 </sst>
 </file>
@@ -1488,11 +1494,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C05FD92-F64B-46B2-B040-D64C583D254F}">
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F72" sqref="F72"/>
+      <selection pane="bottomLeft" activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2744,31 +2750,63 @@
         <v>105</v>
       </c>
       <c r="B72">
-        <v>20616</v>
+        <v>20608</v>
       </c>
       <c r="C72">
         <f t="shared" ref="C72:C73" si="2">B72-B71</f>
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="D72">
         <v>21276</v>
       </c>
       <c r="E72">
         <f t="shared" si="1"/>
-        <v>-660</v>
+        <v>-668</v>
       </c>
       <c r="F72" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>107</v>
+      </c>
+      <c r="B73">
+        <v>20380</v>
+      </c>
       <c r="C73">
         <f t="shared" si="2"/>
-        <v>-20616</v>
+        <v>-228</v>
+      </c>
+      <c r="D73">
+        <v>21276</v>
       </c>
       <c r="E73">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-896</v>
+      </c>
+      <c r="F73" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D74">
+        <v>21276</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D75">
+        <v>21276</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D76">
+        <v>21276</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D77">
+        <v>21276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removing biquad maj7filter removing fold saturation; it's just not useful
</commit_message>
<xml_diff>
--- a/sizework20240216.xlsx
+++ b/sizework20240216.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\root\git\thenfour\WaveSabre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8176A4-FEF8-4A7B-92AC-F0E938F317C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA43D425-26C6-406D-A99A-CC3A8EE2B637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13500" yWindow="1050" windowWidth="19575" windowHeight="16800" activeTab="1" xr2:uid="{0D8D836A-3D74-4865-ACF1-B299F3391987}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="115">
   <si>
     <t>maj7</t>
   </si>
@@ -353,6 +353,24 @@
   </si>
   <si>
     <t>ok now we're talking. Moog is back baby</t>
+  </si>
+  <si>
+    <t>re-adding osc panning</t>
+  </si>
+  <si>
+    <t>oof? Well let's go for it for the moment. I think it's too valuable.</t>
+  </si>
+  <si>
+    <t>without biquad maj7 filter</t>
+  </si>
+  <si>
+    <t>ok fine.</t>
+  </si>
+  <si>
+    <t>so I took some steps back. Let's remove more: sat fold</t>
+  </si>
+  <si>
+    <t>re-adding master pan</t>
   </si>
 </sst>
 </file>
@@ -1494,16 +1512,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C05FD92-F64B-46B2-B040-D64C583D254F}">
-  <dimension ref="A1:F77"/>
+  <dimension ref="A1:F153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A73" sqref="A73"/>
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="62.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1751,7 +1769,7 @@
         <v>21276</v>
       </c>
       <c r="E20">
-        <f t="shared" ref="E20:E73" si="1">B20-D20</f>
+        <f t="shared" ref="E20:E83" si="1">B20-D20</f>
         <v>-36</v>
       </c>
     </row>
@@ -2753,7 +2771,7 @@
         <v>20608</v>
       </c>
       <c r="C72">
-        <f t="shared" ref="C72:C73" si="2">B72-B71</f>
+        <f t="shared" ref="C72:C135" si="2">B72-B71</f>
         <v>332</v>
       </c>
       <c r="D72">
@@ -2790,23 +2808,1073 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>109</v>
+      </c>
+      <c r="B74">
+        <v>20716</v>
+      </c>
+      <c r="C74">
+        <f t="shared" si="2"/>
+        <v>336</v>
+      </c>
       <c r="D74">
         <v>21276</v>
       </c>
+      <c r="E74">
+        <f t="shared" si="1"/>
+        <v>-560</v>
+      </c>
+      <c r="F74" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>111</v>
+      </c>
+      <c r="B75">
+        <v>20672</v>
+      </c>
+      <c r="C75">
+        <f t="shared" si="2"/>
+        <v>-44</v>
+      </c>
       <c r="D75">
         <v>21276</v>
       </c>
+      <c r="E75">
+        <f t="shared" si="1"/>
+        <v>-604</v>
+      </c>
+      <c r="F75" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>113</v>
+      </c>
+      <c r="B76">
+        <v>20632</v>
+      </c>
+      <c r="C76">
+        <f t="shared" si="2"/>
+        <v>-40</v>
+      </c>
       <c r="D76">
         <v>21276</v>
       </c>
+      <c r="E76">
+        <f t="shared" si="1"/>
+        <v>-644</v>
+      </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>114</v>
+      </c>
+      <c r="B77">
+        <v>20660</v>
+      </c>
+      <c r="C77">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
       <c r="D77">
         <v>21276</v>
+      </c>
+      <c r="E77">
+        <f t="shared" si="1"/>
+        <v>-616</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C78">
+        <f t="shared" si="2"/>
+        <v>-20660</v>
+      </c>
+      <c r="D78">
+        <v>21276</v>
+      </c>
+      <c r="E78">
+        <f t="shared" si="1"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C79">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>21276</v>
+      </c>
+      <c r="E79">
+        <f t="shared" si="1"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C80">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>21276</v>
+      </c>
+      <c r="E80">
+        <f t="shared" si="1"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="81" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C81">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>21276</v>
+      </c>
+      <c r="E81">
+        <f t="shared" si="1"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="82" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C82">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D82">
+        <v>21276</v>
+      </c>
+      <c r="E82">
+        <f t="shared" si="1"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="83" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C83">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>21276</v>
+      </c>
+      <c r="E83">
+        <f t="shared" si="1"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="84" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C84">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>21276</v>
+      </c>
+      <c r="E84">
+        <f t="shared" ref="E84:E147" si="3">B84-D84</f>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="85" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C85">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>21276</v>
+      </c>
+      <c r="E85">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="86" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C86">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>21276</v>
+      </c>
+      <c r="E86">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="87" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C87">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>21276</v>
+      </c>
+      <c r="E87">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="88" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C88">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>21276</v>
+      </c>
+      <c r="E88">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="89" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C89">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>21276</v>
+      </c>
+      <c r="E89">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="90" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C90">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>21276</v>
+      </c>
+      <c r="E90">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="91" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C91">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>21276</v>
+      </c>
+      <c r="E91">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="92" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C92">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>21276</v>
+      </c>
+      <c r="E92">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="93" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C93">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>21276</v>
+      </c>
+      <c r="E93">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="94" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C94">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <v>21276</v>
+      </c>
+      <c r="E94">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="95" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C95">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D95">
+        <v>21276</v>
+      </c>
+      <c r="E95">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="96" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C96">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D96">
+        <v>21276</v>
+      </c>
+      <c r="E96">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="97" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C97">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D97">
+        <v>21276</v>
+      </c>
+      <c r="E97">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="98" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C98">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>21276</v>
+      </c>
+      <c r="E98">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="99" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C99">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>21276</v>
+      </c>
+      <c r="E99">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="100" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C100">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D100">
+        <v>21276</v>
+      </c>
+      <c r="E100">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="101" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C101">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>21276</v>
+      </c>
+      <c r="E101">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="102" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C102">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D102">
+        <v>21276</v>
+      </c>
+      <c r="E102">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="103" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C103">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D103">
+        <v>21276</v>
+      </c>
+      <c r="E103">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="104" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C104">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D104">
+        <v>21276</v>
+      </c>
+      <c r="E104">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="105" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C105">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D105">
+        <v>21276</v>
+      </c>
+      <c r="E105">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="106" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C106">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D106">
+        <v>21276</v>
+      </c>
+      <c r="E106">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="107" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C107">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D107">
+        <v>21276</v>
+      </c>
+      <c r="E107">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="108" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C108">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D108">
+        <v>21276</v>
+      </c>
+      <c r="E108">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="109" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C109">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D109">
+        <v>21276</v>
+      </c>
+      <c r="E109">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="110" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C110">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D110">
+        <v>21276</v>
+      </c>
+      <c r="E110">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="111" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C111">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D111">
+        <v>21276</v>
+      </c>
+      <c r="E111">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="112" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C112">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D112">
+        <v>21276</v>
+      </c>
+      <c r="E112">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="113" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C113">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D113">
+        <v>21276</v>
+      </c>
+      <c r="E113">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="114" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C114">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D114">
+        <v>21276</v>
+      </c>
+      <c r="E114">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="115" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C115">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D115">
+        <v>21276</v>
+      </c>
+      <c r="E115">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="116" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C116">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D116">
+        <v>21276</v>
+      </c>
+      <c r="E116">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="117" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C117">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D117">
+        <v>21276</v>
+      </c>
+      <c r="E117">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="118" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C118">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D118">
+        <v>21276</v>
+      </c>
+      <c r="E118">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="119" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C119">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D119">
+        <v>21276</v>
+      </c>
+      <c r="E119">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="120" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C120">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D120">
+        <v>21276</v>
+      </c>
+      <c r="E120">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="121" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C121">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D121">
+        <v>21276</v>
+      </c>
+      <c r="E121">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="122" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C122">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D122">
+        <v>21276</v>
+      </c>
+      <c r="E122">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="123" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C123">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D123">
+        <v>21276</v>
+      </c>
+      <c r="E123">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="124" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C124">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D124">
+        <v>21276</v>
+      </c>
+      <c r="E124">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="125" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C125">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D125">
+        <v>21276</v>
+      </c>
+      <c r="E125">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="126" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C126">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D126">
+        <v>21276</v>
+      </c>
+      <c r="E126">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="127" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C127">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D127">
+        <v>21276</v>
+      </c>
+      <c r="E127">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="128" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C128">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D128">
+        <v>21276</v>
+      </c>
+      <c r="E128">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="129" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C129">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D129">
+        <v>21276</v>
+      </c>
+      <c r="E129">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="130" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C130">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D130">
+        <v>21276</v>
+      </c>
+      <c r="E130">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="131" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C131">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D131">
+        <v>21276</v>
+      </c>
+      <c r="E131">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="132" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C132">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D132">
+        <v>21276</v>
+      </c>
+      <c r="E132">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="133" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C133">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D133">
+        <v>21276</v>
+      </c>
+      <c r="E133">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="134" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C134">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D134">
+        <v>21276</v>
+      </c>
+      <c r="E134">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="135" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C135">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="D135">
+        <v>21276</v>
+      </c>
+      <c r="E135">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="136" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C136">
+        <f t="shared" ref="C136:C153" si="4">B136-B135</f>
+        <v>0</v>
+      </c>
+      <c r="D136">
+        <v>21276</v>
+      </c>
+      <c r="E136">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="137" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C137">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D137">
+        <v>21276</v>
+      </c>
+      <c r="E137">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="138" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C138">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D138">
+        <v>21276</v>
+      </c>
+      <c r="E138">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="139" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C139">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D139">
+        <v>21276</v>
+      </c>
+      <c r="E139">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="140" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C140">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D140">
+        <v>21276</v>
+      </c>
+      <c r="E140">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="141" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C141">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D141">
+        <v>21276</v>
+      </c>
+      <c r="E141">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="142" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C142">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D142">
+        <v>21276</v>
+      </c>
+      <c r="E142">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="143" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C143">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D143">
+        <v>21276</v>
+      </c>
+      <c r="E143">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="144" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C144">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D144">
+        <v>21276</v>
+      </c>
+      <c r="E144">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="145" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C145">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D145">
+        <v>21276</v>
+      </c>
+      <c r="E145">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="146" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C146">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D146">
+        <v>21276</v>
+      </c>
+      <c r="E146">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="147" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C147">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D147">
+        <v>21276</v>
+      </c>
+      <c r="E147">
+        <f t="shared" si="3"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="148" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C148">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D148">
+        <v>21276</v>
+      </c>
+      <c r="E148">
+        <f t="shared" ref="E148:E153" si="5">B148-D148</f>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="149" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C149">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D149">
+        <v>21276</v>
+      </c>
+      <c r="E149">
+        <f t="shared" si="5"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="150" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C150">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D150">
+        <v>21276</v>
+      </c>
+      <c r="E150">
+        <f t="shared" si="5"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="151" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C151">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D151">
+        <v>21276</v>
+      </c>
+      <c r="E151">
+        <f t="shared" si="5"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="152" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C152">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D152">
+        <v>21276</v>
+      </c>
+      <c r="E152">
+        <f t="shared" si="5"/>
+        <v>-21276</v>
+      </c>
+    </row>
+    <row r="153" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C153">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="D153">
+        <v>21276</v>
+      </c>
+      <c r="E153">
+        <f t="shared" si="5"/>
+        <v>-21276</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing crashes when you load presets with OOB enum values loading presets automatically resets amp env modulations
</commit_message>
<xml_diff>
--- a/sizework20240216.xlsx
+++ b/sizework20240216.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\root\git\thenfour\WaveSabre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA43D425-26C6-406D-A99A-CC3A8EE2B637}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34969BE6-B188-4656-8C46-23B8A95AD4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13500" yWindow="1050" windowWidth="19575" windowHeight="16800" activeTab="1" xr2:uid="{0D8D836A-3D74-4865-ACF1-B299F3391987}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="120">
   <si>
     <t>maj7</t>
   </si>
@@ -371,6 +371,21 @@
   </si>
   <si>
     <t>re-adding master pan</t>
+  </si>
+  <si>
+    <t>disabling more sat models + some optimizations in there</t>
+  </si>
+  <si>
+    <t>disabling analog again</t>
+  </si>
+  <si>
+    <t>worth it I guess.</t>
+  </si>
+  <si>
+    <t>some comp optimizations</t>
+  </si>
+  <si>
+    <t>adding chan link param support (I don't think I really meant to remove that)</t>
   </si>
 </sst>
 </file>
@@ -1515,8 +1530,8 @@
   <dimension ref="A1:F153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A77" sqref="A77"/>
+      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2875,76 +2890,103 @@
         <v>114</v>
       </c>
       <c r="B77">
-        <v>20660</v>
+        <v>20672</v>
       </c>
       <c r="C77">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="D77">
         <v>21276</v>
       </c>
       <c r="E77">
         <f t="shared" si="1"/>
-        <v>-616</v>
+        <v>-604</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>115</v>
+      </c>
+      <c r="B78">
+        <v>20620</v>
+      </c>
       <c r="C78">
         <f t="shared" si="2"/>
-        <v>-20660</v>
+        <v>-52</v>
       </c>
       <c r="D78">
         <v>21276</v>
       </c>
       <c r="E78">
         <f t="shared" si="1"/>
-        <v>-21276</v>
+        <v>-656</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>116</v>
+      </c>
+      <c r="B79">
+        <v>20556</v>
+      </c>
       <c r="C79">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-64</v>
       </c>
       <c r="D79">
         <v>21276</v>
       </c>
       <c r="E79">
         <f t="shared" si="1"/>
-        <v>-21276</v>
+        <v>-720</v>
+      </c>
+      <c r="F79" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>118</v>
+      </c>
+      <c r="B80">
+        <v>20532</v>
+      </c>
       <c r="C80">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-24</v>
       </c>
       <c r="D80">
         <v>21276</v>
       </c>
       <c r="E80">
         <f t="shared" si="1"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="81" spans="3:5" x14ac:dyDescent="0.25">
+        <v>-744</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>119</v>
+      </c>
+      <c r="B81">
+        <v>20552</v>
+      </c>
       <c r="C81">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="D81">
         <v>21276</v>
       </c>
       <c r="E81">
         <f t="shared" si="1"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="82" spans="3:5" x14ac:dyDescent="0.25">
+        <v>-724</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C82">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-20552</v>
       </c>
       <c r="D82">
         <v>21276</v>
@@ -2954,7 +2996,7 @@
         <v>-21276</v>
       </c>
     </row>
-    <row r="83" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C83">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2967,7 +3009,7 @@
         <v>-21276</v>
       </c>
     </row>
-    <row r="84" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C84">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2980,7 +3022,7 @@
         <v>-21276</v>
       </c>
     </row>
-    <row r="85" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C85">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -2993,7 +3035,7 @@
         <v>-21276</v>
       </c>
     </row>
-    <row r="86" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C86">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3006,7 +3048,7 @@
         <v>-21276</v>
       </c>
     </row>
-    <row r="87" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C87">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3019,7 +3061,7 @@
         <v>-21276</v>
       </c>
     </row>
-    <row r="88" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C88">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3032,7 +3074,7 @@
         <v>-21276</v>
       </c>
     </row>
-    <row r="89" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C89">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3045,7 +3087,7 @@
         <v>-21276</v>
       </c>
     </row>
-    <row r="90" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C90">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3058,7 +3100,7 @@
         <v>-21276</v>
       </c>
     </row>
-    <row r="91" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C91">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3071,7 +3113,7 @@
         <v>-21276</v>
       </c>
     </row>
-    <row r="92" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C92">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3084,7 +3126,7 @@
         <v>-21276</v>
       </c>
     </row>
-    <row r="93" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C93">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3097,7 +3139,7 @@
         <v>-21276</v>
       </c>
     </row>
-    <row r="94" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C94">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3110,7 +3152,7 @@
         <v>-21276</v>
       </c>
     </row>
-    <row r="95" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C95">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3123,7 +3165,7 @@
         <v>-21276</v>
       </c>
     </row>
-    <row r="96" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C96">
         <f t="shared" si="2"/>
         <v>0</v>

</xml_diff>

<commit_message>
- adding MBC multiband compressor - updating boilerplate for recent changes - adding better support for VST data in json chunk. - sat:   - mute/solo now part of vst chunk but not device.   - many micro optimizations
</commit_message>
<xml_diff>
--- a/sizework20240216.xlsx
+++ b/sizework20240216.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\root\git\thenfour\WaveSabre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34969BE6-B188-4656-8C46-23B8A95AD4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFB3F3B-D218-489A-9D6F-7BD983EE1F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13500" yWindow="1050" windowWidth="19575" windowHeight="16800" activeTab="1" xr2:uid="{0D8D836A-3D74-4865-ACF1-B299F3391987}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="20625" activeTab="1" xr2:uid="{0D8D836A-3D74-4865-ACF1-B299F3391987}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="134">
   <si>
     <t>maj7</t>
   </si>
@@ -386,6 +386,48 @@
   </si>
   <si>
     <t>adding chan link param support (I don't think I really meant to remove that)</t>
+  </si>
+  <si>
+    <t>ok I made a multiband compressor. Before adding it,</t>
+  </si>
+  <si>
+    <t>with MBC</t>
+  </si>
+  <si>
+    <t>wow not bad tbh</t>
+  </si>
+  <si>
+    <t>MBC but not Comp</t>
+  </si>
+  <si>
+    <t>Comp but not MBC</t>
+  </si>
+  <si>
+    <t>with neither</t>
+  </si>
+  <si>
+    <t>so the multiband comp adds 800 bytes to final size</t>
+  </si>
+  <si>
+    <t>normal comp is 450 bytes. So MB does add mor than I expected. I'm going to keep it though.</t>
+  </si>
+  <si>
+    <t>optimizations in sat</t>
+  </si>
+  <si>
+    <t>and considering this is supposed to *replace* comp, readd biquad</t>
+  </si>
+  <si>
+    <t>also optimizations in sat</t>
+  </si>
+  <si>
+    <t>without sat</t>
+  </si>
+  <si>
+    <t>so sat is now 480 bytes of code, that's pretty good tbh</t>
+  </si>
+  <si>
+    <t>something to keep in mind is that sat could be built into MBC</t>
   </si>
 </sst>
 </file>
@@ -1531,7 +1573,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C81" sqref="C81"/>
+      <selection pane="bottomLeft" activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2964,7 +3006,7 @@
         <v>-744</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>119</v>
       </c>
@@ -2983,153 +3025,237 @@
         <v>-724</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>120</v>
+      </c>
+      <c r="B82">
+        <v>20544</v>
+      </c>
       <c r="C82">
         <f t="shared" si="2"/>
-        <v>-20552</v>
+        <v>-8</v>
       </c>
       <c r="D82">
         <v>21276</v>
       </c>
       <c r="E82">
         <f t="shared" si="1"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-732</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>121</v>
+      </c>
+      <c r="B83">
+        <v>20892</v>
+      </c>
       <c r="C83">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>348</v>
       </c>
       <c r="D83">
         <v>21276</v>
       </c>
       <c r="E83">
         <f t="shared" si="1"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-384</v>
+      </c>
+      <c r="F83" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>123</v>
+      </c>
+      <c r="B84">
+        <v>20720</v>
+      </c>
       <c r="C84">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-172</v>
       </c>
       <c r="D84">
         <v>21276</v>
       </c>
       <c r="E84">
         <f t="shared" ref="E84:E147" si="3">B84-D84</f>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-556</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>125</v>
+      </c>
+      <c r="B85">
+        <v>20088</v>
+      </c>
       <c r="C85">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-632</v>
       </c>
       <c r="D85">
         <v>21276</v>
       </c>
       <c r="E85">
         <f t="shared" si="3"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1188</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>121</v>
+      </c>
+      <c r="B86">
+        <v>20892</v>
+      </c>
       <c r="C86">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>804</v>
       </c>
       <c r="D86">
         <v>21276</v>
       </c>
       <c r="E86">
         <f t="shared" si="3"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-384</v>
+      </c>
+      <c r="F86" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>125</v>
+      </c>
+      <c r="B87">
+        <v>20088</v>
+      </c>
       <c r="C87">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-804</v>
       </c>
       <c r="D87">
         <v>21276</v>
       </c>
       <c r="E87">
         <f t="shared" si="3"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1188</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>124</v>
+      </c>
+      <c r="B88">
+        <v>20544</v>
+      </c>
       <c r="C88">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>456</v>
       </c>
       <c r="D88">
         <v>21276</v>
       </c>
       <c r="E88">
         <f t="shared" si="3"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-732</v>
+      </c>
+      <c r="F88" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>123</v>
+      </c>
+      <c r="B89">
+        <v>20720</v>
+      </c>
       <c r="C89">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>176</v>
       </c>
       <c r="D89">
         <v>21276</v>
       </c>
       <c r="E89">
         <f t="shared" si="3"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-556</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>128</v>
+      </c>
+      <c r="B90">
+        <v>20664</v>
+      </c>
       <c r="C90">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-56</v>
       </c>
       <c r="D90">
         <v>21276</v>
       </c>
       <c r="E90">
         <f t="shared" si="3"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-612</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>129</v>
+      </c>
+      <c r="B91">
+        <v>20688</v>
+      </c>
       <c r="C91">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="D91">
         <v>21276</v>
       </c>
       <c r="E91">
         <f t="shared" si="3"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-588</v>
+      </c>
+      <c r="F91" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>131</v>
+      </c>
+      <c r="B92">
+        <v>20204</v>
+      </c>
       <c r="C92">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-484</v>
       </c>
       <c r="D92">
         <v>21276</v>
       </c>
       <c r="E92">
         <f t="shared" si="3"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+        <v>-1072</v>
+      </c>
+      <c r="F92" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>133</v>
+      </c>
       <c r="C93">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-20204</v>
       </c>
       <c r="D93">
         <v>21276</v>
@@ -3139,7 +3265,7 @@
         <v>-21276</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C94">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3152,7 +3278,7 @@
         <v>-21276</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C95">
         <f t="shared" si="2"/>
         <v>0</v>
@@ -3165,7 +3291,7 @@
         <v>-21276</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C96">
         <f t="shared" si="2"/>
         <v>0</v>

</xml_diff>

<commit_message>
echo now has crude echo visualization fixing crash in delaybuffer
</commit_message>
<xml_diff>
--- a/sizework20240216.xlsx
+++ b/sizework20240216.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\root\git\thenfour\WaveSabre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FC4831-6EC0-4581-8C2D-1AB16E14B8F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AE4B3B-89D9-43E5-B815-6A4E445E1AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="20625" activeTab="1" xr2:uid="{0D8D836A-3D74-4865-ACF1-B299F3391987}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="142">
   <si>
     <t>maj7</t>
   </si>
@@ -440,6 +440,18 @@
   </si>
   <si>
     <t>MBC is 1kb of compressed code so that's heavy. But fortunately it does a LOT of work.</t>
+  </si>
+  <si>
+    <t>lots of bug fixes, improvements to filters and echo</t>
+  </si>
+  <si>
+    <t>impressively small change. There were additions + optimizations and apparently mostly balanced out.</t>
+  </si>
+  <si>
+    <t>this is actually the correct baseline</t>
+  </si>
+  <si>
+    <t>so the baseline was after changes; this is a better baseline for the 2023 version. I have added 208 bytes of code. Pretty balanced.</t>
   </si>
 </sst>
 </file>
@@ -819,7 +831,7 @@
   <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1584,8 +1596,8 @@
   <dimension ref="A1:F153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F97" sqref="F97"/>
+      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F100" sqref="F100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3340,212 +3352,233 @@
         <v>137</v>
       </c>
     </row>
-    <row r="97" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B97">
+        <v>20212</v>
+      </c>
       <c r="C97">
         <f t="shared" si="2"/>
-        <v>-19216</v>
+        <v>996</v>
       </c>
       <c r="D97">
         <v>21276</v>
       </c>
       <c r="E97">
         <f t="shared" si="3"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="98" spans="3:5" x14ac:dyDescent="0.25">
+        <v>-1064</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>138</v>
+      </c>
+      <c r="B98">
+        <v>20244</v>
+      </c>
       <c r="C98">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="D98">
         <v>21276</v>
       </c>
       <c r="E98">
         <f t="shared" si="3"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="99" spans="3:5" x14ac:dyDescent="0.25">
+        <v>-1032</v>
+      </c>
+      <c r="F98" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>140</v>
+      </c>
+      <c r="B99">
+        <v>20244</v>
+      </c>
       <c r="C99">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D99">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E99">
         <f t="shared" si="3"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="100" spans="3:5" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+      <c r="F99" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C100">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-20244</v>
       </c>
       <c r="D100">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E100">
         <f t="shared" si="3"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="101" spans="3:5" x14ac:dyDescent="0.25">
+        <v>-20036</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C101">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D101">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E101">
         <f t="shared" si="3"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="102" spans="3:5" x14ac:dyDescent="0.25">
+        <v>-20036</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C102">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D102">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E102">
         <f t="shared" si="3"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="103" spans="3:5" x14ac:dyDescent="0.25">
+        <v>-20036</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C103">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D103">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E103">
         <f t="shared" si="3"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="104" spans="3:5" x14ac:dyDescent="0.25">
+        <v>-20036</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C104">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D104">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E104">
         <f t="shared" si="3"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="105" spans="3:5" x14ac:dyDescent="0.25">
+        <v>-20036</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C105">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D105">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E105">
         <f t="shared" si="3"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="106" spans="3:5" x14ac:dyDescent="0.25">
+        <v>-20036</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C106">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D106">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E106">
         <f t="shared" si="3"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="107" spans="3:5" x14ac:dyDescent="0.25">
+        <v>-20036</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C107">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D107">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E107">
         <f t="shared" si="3"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="108" spans="3:5" x14ac:dyDescent="0.25">
+        <v>-20036</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C108">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D108">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E108">
         <f t="shared" si="3"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="109" spans="3:5" x14ac:dyDescent="0.25">
+        <v>-20036</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C109">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D109">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E109">
         <f t="shared" si="3"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="110" spans="3:5" x14ac:dyDescent="0.25">
+        <v>-20036</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C110">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D110">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E110">
         <f t="shared" si="3"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="111" spans="3:5" x14ac:dyDescent="0.25">
+        <v>-20036</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C111">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D111">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E111">
         <f t="shared" si="3"/>
-        <v>-21276</v>
-      </c>
-    </row>
-    <row r="112" spans="3:5" x14ac:dyDescent="0.25">
+        <v>-20036</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C112">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D112">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E112">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="113" spans="3:5" x14ac:dyDescent="0.25">
@@ -3554,11 +3587,11 @@
         <v>0</v>
       </c>
       <c r="D113">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E113">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="114" spans="3:5" x14ac:dyDescent="0.25">
@@ -3567,11 +3600,11 @@
         <v>0</v>
       </c>
       <c r="D114">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E114">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="115" spans="3:5" x14ac:dyDescent="0.25">
@@ -3580,11 +3613,11 @@
         <v>0</v>
       </c>
       <c r="D115">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E115">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="116" spans="3:5" x14ac:dyDescent="0.25">
@@ -3593,11 +3626,11 @@
         <v>0</v>
       </c>
       <c r="D116">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E116">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="117" spans="3:5" x14ac:dyDescent="0.25">
@@ -3606,11 +3639,11 @@
         <v>0</v>
       </c>
       <c r="D117">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E117">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="118" spans="3:5" x14ac:dyDescent="0.25">
@@ -3619,11 +3652,11 @@
         <v>0</v>
       </c>
       <c r="D118">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E118">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="119" spans="3:5" x14ac:dyDescent="0.25">
@@ -3632,11 +3665,11 @@
         <v>0</v>
       </c>
       <c r="D119">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E119">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="120" spans="3:5" x14ac:dyDescent="0.25">
@@ -3645,11 +3678,11 @@
         <v>0</v>
       </c>
       <c r="D120">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E120">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="121" spans="3:5" x14ac:dyDescent="0.25">
@@ -3658,11 +3691,11 @@
         <v>0</v>
       </c>
       <c r="D121">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E121">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="122" spans="3:5" x14ac:dyDescent="0.25">
@@ -3671,11 +3704,11 @@
         <v>0</v>
       </c>
       <c r="D122">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E122">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="123" spans="3:5" x14ac:dyDescent="0.25">
@@ -3684,11 +3717,11 @@
         <v>0</v>
       </c>
       <c r="D123">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E123">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="124" spans="3:5" x14ac:dyDescent="0.25">
@@ -3697,11 +3730,11 @@
         <v>0</v>
       </c>
       <c r="D124">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E124">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="125" spans="3:5" x14ac:dyDescent="0.25">
@@ -3710,11 +3743,11 @@
         <v>0</v>
       </c>
       <c r="D125">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E125">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="126" spans="3:5" x14ac:dyDescent="0.25">
@@ -3723,11 +3756,11 @@
         <v>0</v>
       </c>
       <c r="D126">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E126">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="127" spans="3:5" x14ac:dyDescent="0.25">
@@ -3736,11 +3769,11 @@
         <v>0</v>
       </c>
       <c r="D127">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E127">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="128" spans="3:5" x14ac:dyDescent="0.25">
@@ -3749,11 +3782,11 @@
         <v>0</v>
       </c>
       <c r="D128">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E128">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="129" spans="3:5" x14ac:dyDescent="0.25">
@@ -3762,11 +3795,11 @@
         <v>0</v>
       </c>
       <c r="D129">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E129">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="130" spans="3:5" x14ac:dyDescent="0.25">
@@ -3775,11 +3808,11 @@
         <v>0</v>
       </c>
       <c r="D130">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E130">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="131" spans="3:5" x14ac:dyDescent="0.25">
@@ -3788,11 +3821,11 @@
         <v>0</v>
       </c>
       <c r="D131">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E131">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="132" spans="3:5" x14ac:dyDescent="0.25">
@@ -3801,11 +3834,11 @@
         <v>0</v>
       </c>
       <c r="D132">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E132">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="133" spans="3:5" x14ac:dyDescent="0.25">
@@ -3814,11 +3847,11 @@
         <v>0</v>
       </c>
       <c r="D133">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E133">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="134" spans="3:5" x14ac:dyDescent="0.25">
@@ -3827,11 +3860,11 @@
         <v>0</v>
       </c>
       <c r="D134">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E134">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="135" spans="3:5" x14ac:dyDescent="0.25">
@@ -3840,11 +3873,11 @@
         <v>0</v>
       </c>
       <c r="D135">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E135">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="136" spans="3:5" x14ac:dyDescent="0.25">
@@ -3853,11 +3886,11 @@
         <v>0</v>
       </c>
       <c r="D136">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E136">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="137" spans="3:5" x14ac:dyDescent="0.25">
@@ -3866,11 +3899,11 @@
         <v>0</v>
       </c>
       <c r="D137">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E137">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="138" spans="3:5" x14ac:dyDescent="0.25">
@@ -3879,11 +3912,11 @@
         <v>0</v>
       </c>
       <c r="D138">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E138">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="139" spans="3:5" x14ac:dyDescent="0.25">
@@ -3892,11 +3925,11 @@
         <v>0</v>
       </c>
       <c r="D139">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E139">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="140" spans="3:5" x14ac:dyDescent="0.25">
@@ -3905,11 +3938,11 @@
         <v>0</v>
       </c>
       <c r="D140">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E140">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="141" spans="3:5" x14ac:dyDescent="0.25">
@@ -3918,11 +3951,11 @@
         <v>0</v>
       </c>
       <c r="D141">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E141">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="142" spans="3:5" x14ac:dyDescent="0.25">
@@ -3931,11 +3964,11 @@
         <v>0</v>
       </c>
       <c r="D142">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E142">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="143" spans="3:5" x14ac:dyDescent="0.25">
@@ -3944,11 +3977,11 @@
         <v>0</v>
       </c>
       <c r="D143">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E143">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="144" spans="3:5" x14ac:dyDescent="0.25">
@@ -3957,11 +3990,11 @@
         <v>0</v>
       </c>
       <c r="D144">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E144">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="145" spans="3:5" x14ac:dyDescent="0.25">
@@ -3970,11 +4003,11 @@
         <v>0</v>
       </c>
       <c r="D145">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E145">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="146" spans="3:5" x14ac:dyDescent="0.25">
@@ -3983,11 +4016,11 @@
         <v>0</v>
       </c>
       <c r="D146">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E146">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="147" spans="3:5" x14ac:dyDescent="0.25">
@@ -3996,11 +4029,11 @@
         <v>0</v>
       </c>
       <c r="D147">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E147">
         <f t="shared" si="3"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="148" spans="3:5" x14ac:dyDescent="0.25">
@@ -4009,11 +4042,11 @@
         <v>0</v>
       </c>
       <c r="D148">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E148">
         <f t="shared" ref="E148:E153" si="5">B148-D148</f>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="149" spans="3:5" x14ac:dyDescent="0.25">
@@ -4022,11 +4055,11 @@
         <v>0</v>
       </c>
       <c r="D149">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E149">
         <f t="shared" si="5"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="150" spans="3:5" x14ac:dyDescent="0.25">
@@ -4035,11 +4068,11 @@
         <v>0</v>
       </c>
       <c r="D150">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E150">
         <f t="shared" si="5"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="151" spans="3:5" x14ac:dyDescent="0.25">
@@ -4048,11 +4081,11 @@
         <v>0</v>
       </c>
       <c r="D151">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E151">
         <f t="shared" si="5"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="152" spans="3:5" x14ac:dyDescent="0.25">
@@ -4061,11 +4094,11 @@
         <v>0</v>
       </c>
       <c r="D152">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E152">
         <f t="shared" si="5"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
     <row r="153" spans="3:5" x14ac:dyDescent="0.25">
@@ -4074,11 +4107,11 @@
         <v>0</v>
       </c>
       <c r="D153">
-        <v>21276</v>
+        <v>20036</v>
       </c>
       <c r="E153">
         <f t="shared" si="5"/>
-        <v>-21276</v>
+        <v>-20036</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#69 cathedral comb filter had uninitialized value adding vu meters to cathedral better default values for cathedral roomsize fixed param curve removed freeze & width; they are not helpful and can be worked-around if you need them. unifying audio buffers to AudioBuffer class.
</commit_message>
<xml_diff>
--- a/sizework20240216.xlsx
+++ b/sizework20240216.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\root\git\thenfour\WaveSabre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AE4B3B-89D9-43E5-B815-6A4E445E1AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5719734-1CB2-433B-BB9D-53FCA278728E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="20625" activeTab="1" xr2:uid="{0D8D836A-3D74-4865-ACF1-B299F3391987}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="145">
   <si>
     <t>maj7</t>
   </si>
@@ -452,6 +452,15 @@
   </si>
   <si>
     <t>so the baseline was after changes; this is a better baseline for the 2023 version. I have added 208 bytes of code. Pretty balanced.</t>
+  </si>
+  <si>
+    <t>more bug fixes, removing redundant code</t>
+  </si>
+  <si>
+    <t>removing cathedral freeze, width, unifying delay buffers.</t>
+  </si>
+  <si>
+    <t>well it's helpful but I expected better.</t>
   </si>
 </sst>
 </file>
@@ -1596,8 +1605,8 @@
   <dimension ref="A1:F153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A67" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F100" sqref="F100"/>
+      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3413,35 +3422,50 @@
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>142</v>
+      </c>
+      <c r="B100">
+        <v>20176</v>
+      </c>
       <c r="C100">
         <f t="shared" si="2"/>
-        <v>-20244</v>
+        <v>-68</v>
       </c>
       <c r="D100">
         <v>20036</v>
       </c>
       <c r="E100">
         <f t="shared" si="3"/>
-        <v>-20036</v>
+        <v>140</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>143</v>
+      </c>
+      <c r="B101">
+        <v>20056</v>
+      </c>
       <c r="C101">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="D101">
         <v>20036</v>
       </c>
       <c r="E101">
         <f t="shared" si="3"/>
-        <v>-20036</v>
+        <v>20</v>
+      </c>
+      <c r="F101" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C102">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-20056</v>
       </c>
       <c r="D102">
         <v>20036</v>

</xml_diff>

<commit_message>
fixing biquad Q params in Echo, MBC adding soft clipping options to MBC for mastering - #73 MBC hides bands when in single band mode
</commit_message>
<xml_diff>
--- a/sizework20240216.xlsx
+++ b/sizework20240216.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\root\git\thenfour\WaveSabre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1622364-606B-4F54-8D38-3828D1D84823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5EC7B9B-4230-46FF-8C8E-8EE9F116B37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="20625" activeTab="1" xr2:uid="{0D8D836A-3D74-4865-ACF1-B299F3391987}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="148">
   <si>
     <t>maj7</t>
   </si>
@@ -467,6 +467,9 @@
   </si>
   <si>
     <t>man I would LOVE to shave off 50 bytes to bring to parity with 2023.</t>
+  </si>
+  <si>
+    <t>fixing bugs in synth device - adding cs and changing event buf max</t>
   </si>
 </sst>
 </file>
@@ -1612,7 +1615,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B102" sqref="B102"/>
+      <selection pane="bottomLeft" activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3491,22 +3494,28 @@
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>147</v>
+      </c>
+      <c r="B103">
+        <v>20140</v>
+      </c>
       <c r="C103">
         <f t="shared" si="2"/>
-        <v>-20080</v>
+        <v>60</v>
       </c>
       <c r="D103">
         <v>20036</v>
       </c>
       <c r="E103">
         <f t="shared" si="3"/>
-        <v>-20036</v>
+        <v>104</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C104">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-20140</v>
       </c>
       <c r="D104">
         <v>20036</v>

</xml_diff>

<commit_message>
hiding more stuff in MBC editor when disabled; less distracting. fixing manual frequency input tweaks to mbc params
</commit_message>
<xml_diff>
--- a/sizework20240216.xlsx
+++ b/sizework20240216.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\root\git\thenfour\WaveSabre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5EC7B9B-4230-46FF-8C8E-8EE9F116B37D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520780D4-37F3-4496-9DF7-AFEFA2EDD8D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="20625" activeTab="1" xr2:uid="{0D8D836A-3D74-4865-ACF1-B299F3391987}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="149">
   <si>
     <t>maj7</t>
   </si>
@@ -470,6 +470,9 @@
   </si>
   <si>
     <t>fixing bugs in synth device - adding cs and changing event buf max</t>
+  </si>
+  <si>
+    <t>adding limiter to mbc. It was really missing</t>
   </si>
 </sst>
 </file>
@@ -1615,7 +1618,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B103" sqref="B103"/>
+      <selection pane="bottomLeft" activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3513,22 +3516,28 @@
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>148</v>
+      </c>
+      <c r="B104">
+        <v>20232</v>
+      </c>
       <c r="C104">
         <f t="shared" si="2"/>
-        <v>-20140</v>
+        <v>92</v>
       </c>
       <c r="D104">
         <v>20036</v>
       </c>
       <c r="E104">
         <f t="shared" si="3"/>
-        <v>-20036</v>
+        <v>196</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C105">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-20232</v>
       </c>
       <c r="D105">
         <v>20036</v>

</xml_diff>

<commit_message>
adding docs for MBC adding small, normal, big display modes to MBC editor fixing echo default values fixing MBC default values display tweaks
</commit_message>
<xml_diff>
--- a/sizework20240216.xlsx
+++ b/sizework20240216.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\root\git\thenfour\WaveSabre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520780D4-37F3-4496-9DF7-AFEFA2EDD8D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B45A4A-1A39-4FCB-A192-8710DAA3B2E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="20625" activeTab="1" xr2:uid="{0D8D836A-3D74-4865-ACF1-B299F3391987}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="150">
   <si>
     <t>maj7</t>
   </si>
@@ -473,6 +473,9 @@
   </si>
   <si>
     <t>adding limiter to mbc. It was really missing</t>
+  </si>
+  <si>
+    <t>adding drive gain compensation</t>
   </si>
 </sst>
 </file>
@@ -1618,7 +1621,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A105" sqref="A105"/>
+      <selection pane="bottomLeft" activeCell="A106" sqref="A106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3535,22 +3538,28 @@
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>149</v>
+      </c>
+      <c r="B105">
+        <v>20252</v>
+      </c>
       <c r="C105">
         <f t="shared" si="2"/>
-        <v>-20232</v>
+        <v>20</v>
       </c>
       <c r="D105">
         <v>20036</v>
       </c>
       <c r="E105">
         <f t="shared" si="3"/>
-        <v>-20036</v>
+        <v>216</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C106">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-20252</v>
       </c>
       <c r="D106">
         <v>20036</v>

</xml_diff>

<commit_message>
code cleanups project manager: improvements to project details, better warnings prelim tempo map parsing crusher is officially out
</commit_message>
<xml_diff>
--- a/sizework20240216.xlsx
+++ b/sizework20240216.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\root\git\thenfour\WaveSabre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B45A4A-1A39-4FCB-A192-8710DAA3B2E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87645CCF-F837-467F-B898-4849B21D6865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="20625" activeTab="1" xr2:uid="{0D8D836A-3D74-4865-ACF1-B299F3391987}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="20625" activeTab="2" xr2:uid="{0D8D836A-3D74-4865-ACF1-B299F3391987}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="156">
   <si>
     <t>maj7</t>
   </si>
@@ -476,6 +477,24 @@
   </si>
   <si>
     <t>adding drive gain compensation</t>
+  </si>
+  <si>
+    <t>current size</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>remaining</t>
+  </si>
+  <si>
+    <t>adding fixedvel etc</t>
+  </si>
+  <si>
+    <t>fixing broken things in the payload</t>
+  </si>
+  <si>
+    <t>merge dog bark track</t>
   </si>
 </sst>
 </file>
@@ -1619,7 +1638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C05FD92-F64B-46B2-B040-D64C583D254F}">
   <dimension ref="A1:F153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A106" sqref="A106"/>
     </sheetView>
@@ -4183,4 +4202,247 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA48D90-71FD-4A1F-87C1-A98C78802BBB}">
+  <dimension ref="A1:D30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="101.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>15343</v>
+      </c>
+      <c r="B2">
+        <v>14000</v>
+      </c>
+      <c r="C2">
+        <f>A2-B2</f>
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>15135</v>
+      </c>
+      <c r="B3">
+        <v>14000</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C30" si="0">A3-B3</f>
+        <v>1135</v>
+      </c>
+      <c r="D3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>15318</v>
+      </c>
+      <c r="B4">
+        <v>14000</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>1318</v>
+      </c>
+      <c r="D4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>15306</v>
+      </c>
+      <c r="B5">
+        <v>14000</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>1306</v>
+      </c>
+      <c r="D5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>14000</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{146425CA-02BF-4B94-99D8-CC03B9D4A743}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{146425CA-02BF-4B94-99D8-CC03B9D4A743}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C1:C1048576</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
#107: addressing timestamp serialization and scaling thereof #106: removing pitch bend & CC support #96: notes are serialized as noteon/off pairs with configurable timestamp scale - automation lane points are also now interleaved and timestamps scaled #89: (WIP) hard-code size-optimized samplerate for size opt (also removing from song payload) - removing 8-byte header in song payload - removing support for one-shots because it was causing issues i didn't want to debug. project manager: - logging now outputs to debug & console
</commit_message>
<xml_diff>
--- a/sizework20240216.xlsx
+++ b/sizework20240216.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\root\git\thenfour\WaveSabre\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87645CCF-F837-467F-B898-4849B21D6865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39F17850-F715-486F-BBD3-9F31319F68B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="20625" activeTab="2" xr2:uid="{0D8D836A-3D74-4865-ACF1-B299F3391987}"/>
+    <workbookView xWindow="17760" yWindow="4740" windowWidth="19575" windowHeight="14400" activeTab="1" xr2:uid="{0D8D836A-3D74-4865-ACF1-B299F3391987}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="161">
   <si>
     <t>maj7</t>
   </si>
@@ -495,6 +495,21 @@
   </si>
   <si>
     <t>merge dog bark track</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>4,128 quant new format of midi</t>
+  </si>
+  <si>
+    <t>with new automation point interleave</t>
+  </si>
+  <si>
+    <t>automation point timestamp scaling</t>
+  </si>
+  <si>
+    <t>1,128 quant, no oneshot support</t>
   </si>
 </sst>
 </file>
@@ -550,13 +565,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1638,7 +1654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C05FD92-F64B-46B2-B040-D64C583D254F}">
   <dimension ref="A1:F153"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A106" sqref="A106"/>
     </sheetView>
@@ -4206,18 +4222,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CA48D90-71FD-4A1F-87C1-A98C78802BBB}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="101.140625" customWidth="1"/>
+    <col min="4" max="4" width="101.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>150</v>
       </c>
@@ -4225,22 +4241,25 @@
         <v>151</v>
       </c>
       <c r="C1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>15343</v>
       </c>
       <c r="B2">
         <v>14000</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <f>A2-B2</f>
         <v>1343</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>15135</v>
       </c>
@@ -4248,14 +4267,18 @@
         <v>14000</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C30" si="0">A3-B3</f>
+        <f>A3-A2</f>
+        <v>-208</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D11" si="0">A3-B3</f>
         <v>1135</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>15318</v>
       </c>
@@ -4263,14 +4286,18 @@
         <v>14000</v>
       </c>
       <c r="C4">
+        <f t="shared" ref="C4:C30" si="1">A4-A3</f>
+        <v>183</v>
+      </c>
+      <c r="D4">
         <f t="shared" si="0"/>
         <v>1318</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>15306</v>
       </c>
@@ -4278,64 +4305,142 @@
         <v>14000</v>
       </c>
       <c r="C5">
+        <f t="shared" si="1"/>
+        <v>-12</v>
+      </c>
+      <c r="D5">
         <f t="shared" si="0"/>
         <v>1306</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>13283</v>
+      </c>
       <c r="B6">
         <v>14000</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>-2023</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>-717</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>13265</v>
+      </c>
       <c r="B7">
         <v>14000</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>-18</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>-735</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>13037</v>
+      </c>
       <c r="B8">
         <v>14000</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>-228</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>-963</v>
+      </c>
+      <c r="E8" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>13014</v>
+      </c>
       <c r="B9">
         <v>14000</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>-23</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>-986</v>
+      </c>
+      <c r="E9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>12975</v>
+      </c>
       <c r="B10">
         <v>14000</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>-39</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>-1025</v>
+      </c>
+      <c r="E10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>13382</v>
+      </c>
       <c r="B11">
         <v>14000</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>-618</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>14000</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>14000</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>14000</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>14000</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>14000</v>
       </c>
@@ -4411,7 +4516,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C1048576">
+  <conditionalFormatting sqref="D1:D1048576">
     <cfRule type="dataBar" priority="1">
       <dataBar>
         <cfvo type="min"/>
@@ -4439,7 +4544,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>C1:C1048576</xm:sqref>
+          <xm:sqref>D1:D1048576</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>